<commit_message>
Added date to my text and updated csv files for NA into blanks
</commit_message>
<xml_diff>
--- a/GreenIguanaMasterSpring2021.xlsx
+++ b/GreenIguanaMasterSpring2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usu-my.sharepoint.com/personal/a02308724_aggies_usu_edu/Documents/Desktop/ASU green iguana 2021/greeniguanaAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3E1F204-3744-4711-9BBE-5D795E9D066E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="181" documentId="8_{D3E1F204-3744-4711-9BBE-5D795E9D066E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDEAD138-3C9C-45A1-898F-D862980AC593}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-1470" windowWidth="25440" windowHeight="15390" xr2:uid="{480D2B5B-0BF7-4EFB-BBDF-5EF1CCA213B8}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="221">
   <si>
     <t>0324bka</t>
   </si>
@@ -1094,8 +1094,8 @@
   <dimension ref="A1:FW37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E8" sqref="E8"/>
+      <pane xSplit="1" topLeftCell="FB1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="FO21" sqref="FO21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1825,12 +1825,6 @@
       <c r="BH2">
         <v>2.6666666666666665</v>
       </c>
-      <c r="BI2" t="s">
-        <v>1</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>1</v>
-      </c>
       <c r="BK2">
         <v>2.6666666666666665</v>
       </c>
@@ -1864,12 +1858,6 @@
       <c r="BU2">
         <v>0</v>
       </c>
-      <c r="BV2" t="s">
-        <v>1</v>
-      </c>
-      <c r="BW2" t="s">
-        <v>1</v>
-      </c>
       <c r="BX2">
         <v>6.2156505040806529</v>
       </c>
@@ -1903,9 +1891,6 @@
       <c r="CH2">
         <v>19.947420147420146</v>
       </c>
-      <c r="CI2" t="s">
-        <v>1</v>
-      </c>
       <c r="CJ2">
         <v>28.914987714987713</v>
       </c>
@@ -1942,9 +1927,6 @@
       <c r="CU2">
         <v>326.41810918774974</v>
       </c>
-      <c r="CV2" t="s">
-        <v>1</v>
-      </c>
       <c r="CW2">
         <v>343.026706231454</v>
       </c>
@@ -1981,9 +1963,6 @@
       <c r="DH2">
         <v>6.7555555555555555</v>
       </c>
-      <c r="DI2" t="s">
-        <v>1</v>
-      </c>
       <c r="DJ2">
         <v>6.2391752577319579</v>
       </c>
@@ -2020,9 +1999,6 @@
       <c r="DU2">
         <v>3.5917242450120339</v>
       </c>
-      <c r="DV2" t="s">
-        <v>1</v>
-      </c>
       <c r="DW2">
         <v>2.7308447937131626</v>
       </c>
@@ -2059,9 +2035,6 @@
       <c r="EH2">
         <v>4.0393470071159481</v>
       </c>
-      <c r="EI2" t="s">
-        <v>1</v>
-      </c>
       <c r="EJ2">
         <v>4.6923417441345734</v>
       </c>
@@ -2098,9 +2071,6 @@
       <c r="EU2">
         <v>0.96229087869852048</v>
       </c>
-      <c r="EV2" t="s">
-        <v>1</v>
-      </c>
       <c r="EW2">
         <v>2.0516843384472456</v>
       </c>
@@ -2136,9 +2106,6 @@
       </c>
       <c r="FH2">
         <v>-7.6118429368162183E-2</v>
-      </c>
-      <c r="FI2" t="s">
-        <v>1</v>
       </c>
       <c r="FJ2">
         <v>4.5789074579987009E-2</v>
@@ -2186,9 +2153,6 @@
       <c r="FU2">
         <f t="shared" si="0"/>
         <v>1.0384093080666827</v>
-      </c>
-      <c r="FV2" t="s">
-        <v>1</v>
       </c>
       <c r="FW2">
         <f t="shared" si="0"/>
@@ -2907,9 +2871,6 @@
       <c r="BA4">
         <v>0</v>
       </c>
-      <c r="BB4" s="6" t="s">
-        <v>1</v>
-      </c>
       <c r="BC4">
         <v>0</v>
       </c>
@@ -2946,9 +2907,6 @@
       <c r="BN4">
         <v>0.33333333333333331</v>
       </c>
-      <c r="BO4" s="9" t="s">
-        <v>1</v>
-      </c>
       <c r="BP4">
         <v>0</v>
       </c>
@@ -3051,9 +3009,6 @@
       <c r="CW4">
         <v>354.12462908011872</v>
       </c>
-      <c r="CX4" t="s">
-        <v>1</v>
-      </c>
       <c r="CY4">
         <v>4.7627118644067794</v>
       </c>
@@ -3090,9 +3045,6 @@
       <c r="DJ4">
         <v>3.8886597938144325</v>
       </c>
-      <c r="DK4" t="s">
-        <v>1</v>
-      </c>
       <c r="DL4">
         <v>3.7417986877900473</v>
       </c>
@@ -3128,9 +3080,6 @@
       </c>
       <c r="DW4">
         <v>3.4506876227897831</v>
-      </c>
-      <c r="DX4" t="s">
-        <v>1</v>
       </c>
       <c r="DY4">
         <v>1.1297493936944218</v>
@@ -3612,9 +3561,6 @@
       <c r="CZ5">
         <v>1.3495904690990317</v>
       </c>
-      <c r="DA5" t="s">
-        <v>1</v>
-      </c>
       <c r="DB5">
         <v>5.385618479880776</v>
       </c>
@@ -3651,9 +3597,6 @@
       <c r="DM5">
         <v>1.0340572556762093</v>
       </c>
-      <c r="DN5" t="s">
-        <v>1</v>
-      </c>
       <c r="DO5">
         <v>2.6977140423115156</v>
       </c>
@@ -3689,9 +3632,6 @@
       </c>
       <c r="DZ5">
         <v>0.51884959191605118</v>
-      </c>
-      <c r="EA5" t="s">
-        <v>1</v>
       </c>
       <c r="EB5">
         <v>3.5097656250000004</v>
@@ -4026,9 +3966,6 @@
       <c r="BF6">
         <v>4</v>
       </c>
-      <c r="BG6" t="s">
-        <v>1</v>
-      </c>
       <c r="BH6">
         <v>2.3333333333333335</v>
       </c>
@@ -4065,9 +4002,6 @@
       <c r="BS6">
         <v>2.3333333333333335</v>
       </c>
-      <c r="BT6" t="s">
-        <v>1</v>
-      </c>
       <c r="BU6">
         <v>1.6666666666666667</v>
       </c>
@@ -4182,9 +4116,6 @@
       <c r="DF6">
         <v>3.9519408502772642</v>
       </c>
-      <c r="DG6" t="s">
-        <v>1</v>
-      </c>
       <c r="DH6">
         <v>3.6101010101010105</v>
       </c>
@@ -4221,9 +4152,6 @@
       <c r="DS6">
         <v>1.9103889709502699</v>
       </c>
-      <c r="DT6" t="s">
-        <v>1</v>
-      </c>
       <c r="DU6">
         <v>2.5293067308438788</v>
       </c>
@@ -4260,9 +4188,6 @@
       <c r="EF6">
         <v>2.7459819678557427</v>
       </c>
-      <c r="EG6" t="s">
-        <v>1</v>
-      </c>
       <c r="EH6">
         <v>1.3980745081624113</v>
       </c>
@@ -4337,9 +4262,6 @@
       </c>
       <c r="FF6">
         <v>-1.2974618853610975</v>
-      </c>
-      <c r="FG6" t="s">
-        <v>1</v>
       </c>
       <c r="FH6">
         <v>-3.9087842107976438E-2</v>
@@ -4385,9 +4307,6 @@
       <c r="FS6">
         <f t="shared" si="0"/>
         <v>2.2015592366786443</v>
-      </c>
-      <c r="FT6" t="s">
-        <v>1</v>
       </c>
       <c r="FU6">
         <f t="shared" si="0"/>
@@ -4559,9 +4478,6 @@
       <c r="AZ7">
         <v>0</v>
       </c>
-      <c r="BA7" t="s">
-        <v>1</v>
-      </c>
       <c r="BB7" s="6">
         <v>0</v>
       </c>
@@ -5138,9 +5054,6 @@
       <c r="BI8">
         <v>0.33333333333333331</v>
       </c>
-      <c r="BJ8" t="s">
-        <v>1</v>
-      </c>
       <c r="BK8">
         <v>2</v>
       </c>
@@ -5177,9 +5090,6 @@
       <c r="BV8">
         <v>0.66666666666666663</v>
       </c>
-      <c r="BW8" t="s">
-        <v>1</v>
-      </c>
       <c r="BX8">
         <v>4.5488238118098892</v>
       </c>
@@ -5255,9 +5165,6 @@
       <c r="CV8">
         <v>349.080118694362</v>
       </c>
-      <c r="CW8" t="s">
-        <v>1</v>
-      </c>
       <c r="CX8">
         <v>1.9088983050847457</v>
       </c>
@@ -5449,9 +5356,6 @@
       </c>
       <c r="FI8">
         <v>0.58188606457855419</v>
-      </c>
-      <c r="FJ8" t="s">
-        <v>1</v>
       </c>
       <c r="FK8">
         <f t="shared" si="1"/>
@@ -5500,9 +5404,6 @@
       <c r="FV8">
         <f t="shared" si="0"/>
         <v>-1.2826825384337956</v>
-      </c>
-      <c r="FW8" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:179" x14ac:dyDescent="0.35">
@@ -6172,9 +6073,6 @@
       <c r="AL10">
         <v>71.1011459890384</v>
       </c>
-      <c r="AM10" t="s">
-        <v>1</v>
-      </c>
       <c r="AN10">
         <v>67.588932806324081</v>
       </c>
@@ -6205,9 +6103,6 @@
       <c r="AW10">
         <v>88.222083593262639</v>
       </c>
-      <c r="AX10" t="s">
-        <v>1</v>
-      </c>
       <c r="AY10">
         <v>2</v>
       </c>
@@ -6235,24 +6130,15 @@
       <c r="BG10">
         <v>1.3333333333333333</v>
       </c>
-      <c r="BH10" t="s">
-        <v>1</v>
-      </c>
       <c r="BI10">
         <v>3.3333333333333335</v>
       </c>
       <c r="BJ10">
         <v>0.66666666666666663</v>
       </c>
-      <c r="BK10" t="s">
-        <v>1</v>
-      </c>
       <c r="BL10">
         <v>2.6666666666666665</v>
       </c>
-      <c r="BM10" t="s">
-        <v>1</v>
-      </c>
       <c r="BN10">
         <v>0.66666666666666663</v>
       </c>
@@ -6274,9 +6160,6 @@
       <c r="BT10">
         <v>0</v>
       </c>
-      <c r="BU10" t="s">
-        <v>1</v>
-      </c>
       <c r="BV10">
         <v>0</v>
       </c>
@@ -6289,9 +6172,6 @@
       <c r="BY10">
         <v>3.2012810248198562</v>
       </c>
-      <c r="BZ10" t="s">
-        <v>1</v>
-      </c>
       <c r="CA10">
         <v>12.424755700325733</v>
       </c>
@@ -6328,9 +6208,6 @@
       <c r="CL10">
         <v>342.54443405051455</v>
       </c>
-      <c r="CM10" t="s">
-        <v>1</v>
-      </c>
       <c r="CN10">
         <v>328.61491628614914</v>
       </c>
@@ -6361,15 +6238,9 @@
       <c r="CW10">
         <v>349.080118694362</v>
       </c>
-      <c r="CX10" t="s">
-        <v>1</v>
-      </c>
       <c r="CY10">
         <v>2.7076271186440684</v>
       </c>
-      <c r="CZ10" t="s">
-        <v>1</v>
-      </c>
       <c r="DA10">
         <v>2.6387176325524053</v>
       </c>
@@ -6400,15 +6271,9 @@
       <c r="DJ10">
         <v>2.6680412371134015</v>
       </c>
-      <c r="DK10" t="s">
-        <v>1</v>
-      </c>
       <c r="DL10">
         <v>2.5952152344375099</v>
       </c>
-      <c r="DM10" t="s">
-        <v>1</v>
-      </c>
       <c r="DN10">
         <v>2.3125440727101783</v>
       </c>
@@ -6439,15 +6304,9 @@
       <c r="DW10">
         <v>1.9324165029469544</v>
       </c>
-      <c r="DX10" t="s">
-        <v>1</v>
-      </c>
       <c r="DY10">
         <v>0.1273241713823767</v>
       </c>
-      <c r="DZ10" t="s">
-        <v>1</v>
-      </c>
       <c r="EA10">
         <v>0.44776119402985082</v>
       </c>
@@ -6484,9 +6343,6 @@
       <c r="EL10">
         <v>-0.95797550008366683</v>
       </c>
-      <c r="EM10" t="s">
-        <v>1</v>
-      </c>
       <c r="EN10">
         <v>-0.15303463027279826</v>
       </c>
@@ -6522,9 +6378,6 @@
       </c>
       <c r="EY10">
         <v>0.97355140418608987</v>
-      </c>
-      <c r="EZ10" t="s">
-        <v>1</v>
       </c>
       <c r="FA10">
         <v>-1.1628418426879035</v>
@@ -6563,9 +6416,6 @@
       <c r="FL10">
         <f t="shared" si="0"/>
         <v>-1.9315269042697567</v>
-      </c>
-      <c r="FM10" t="s">
-        <v>1</v>
       </c>
       <c r="FN10">
         <f t="shared" si="0"/>
@@ -6756,9 +6606,6 @@
       <c r="AW11">
         <v>82.956955708047417</v>
       </c>
-      <c r="AX11" t="s">
-        <v>1</v>
-      </c>
       <c r="AY11">
         <v>2</v>
       </c>
@@ -6768,15 +6615,7 @@
       <c r="BA11">
         <v>2</v>
       </c>
-      <c r="BB11" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="BC11" t="s">
-        <v>1</v>
-      </c>
-      <c r="BD11" t="s">
-        <v>1</v>
-      </c>
+      <c r="BB11" s="7"/>
       <c r="BE11">
         <v>3</v>
       </c>
@@ -6795,9 +6634,6 @@
       <c r="BJ11">
         <v>4</v>
       </c>
-      <c r="BK11" t="s">
-        <v>1</v>
-      </c>
       <c r="BL11">
         <v>1.3333333333333333</v>
       </c>
@@ -6807,15 +6643,6 @@
       <c r="BN11">
         <v>1.6666666666666667</v>
       </c>
-      <c r="BO11" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="BP11" t="s">
-        <v>1</v>
-      </c>
-      <c r="BQ11" t="s">
-        <v>1</v>
-      </c>
       <c r="BR11">
         <v>2.3333333333333335</v>
       </c>
@@ -6849,9 +6676,6 @@
       <c r="CB11">
         <v>14.549126213592231</v>
       </c>
-      <c r="CC11" t="s">
-        <v>1</v>
-      </c>
       <c r="CD11">
         <v>17.034730538922155</v>
       </c>
@@ -6912,9 +6736,6 @@
       <c r="CW11">
         <v>338.486646884273</v>
       </c>
-      <c r="CX11" t="s">
-        <v>1</v>
-      </c>
       <c r="CY11">
         <v>1.7926284437825761</v>
       </c>
@@ -6927,12 +6748,6 @@
       <c r="DB11">
         <v>6.0674366616989577</v>
       </c>
-      <c r="DC11" t="s">
-        <v>1</v>
-      </c>
-      <c r="DD11" t="s">
-        <v>1</v>
-      </c>
       <c r="DE11">
         <v>1.5510033444816054</v>
       </c>
@@ -6951,9 +6766,6 @@
       <c r="DJ11">
         <v>5.3402061855670091</v>
       </c>
-      <c r="DK11" t="s">
-        <v>1</v>
-      </c>
       <c r="DL11">
         <v>1.1236073896488505</v>
       </c>
@@ -6966,12 +6778,6 @@
       <c r="DO11">
         <v>1.9757205736191956</v>
       </c>
-      <c r="DP11" t="s">
-        <v>1</v>
-      </c>
-      <c r="DQ11" t="s">
-        <v>1</v>
-      </c>
       <c r="DR11">
         <v>1.2537632704801138</v>
       </c>
@@ -6990,9 +6796,6 @@
       <c r="DW11">
         <v>3.9850687622789778</v>
       </c>
-      <c r="DX11" t="s">
-        <v>1</v>
-      </c>
       <c r="DY11">
         <v>0.97357170617955724</v>
       </c>
@@ -7005,12 +6808,6 @@
       <c r="EB11">
         <v>5.396484375</v>
       </c>
-      <c r="EC11" t="s">
-        <v>1</v>
-      </c>
-      <c r="ED11" t="s">
-        <v>1</v>
-      </c>
       <c r="EE11">
         <v>0.48558758314855888</v>
       </c>
@@ -7043,9 +6840,6 @@
       </c>
       <c r="EO11">
         <v>-0.32963349033073369</v>
-      </c>
-      <c r="EP11" t="s">
-        <v>1</v>
       </c>
       <c r="EQ11">
         <v>0.8771933031205682</v>
@@ -7126,9 +6920,6 @@
       <c r="FO11">
         <f t="shared" si="0"/>
         <v>-1.8267648461785442</v>
-      </c>
-      <c r="FP11" t="s">
-        <v>1</v>
       </c>
       <c r="FQ11">
         <f t="shared" si="0"/>
@@ -7319,9 +7110,7 @@
       <c r="BA12">
         <v>0</v>
       </c>
-      <c r="BB12" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="BB12" s="7"/>
       <c r="BC12">
         <v>1</v>
       </c>
@@ -7357,9 +7146,6 @@
       </c>
       <c r="BN12">
         <v>0.33333333333333331</v>
-      </c>
-      <c r="BO12" s="9" t="s">
-        <v>1</v>
       </c>
       <c r="BP12">
         <v>0.33333333333333331</v>
@@ -7862,24 +7648,15 @@
       <c r="AX13">
         <v>2</v>
       </c>
-      <c r="AY13" t="s">
-        <v>1</v>
-      </c>
       <c r="AZ13">
         <v>1</v>
       </c>
       <c r="BA13">
         <v>0</v>
       </c>
-      <c r="BB13" s="6" t="s">
-        <v>1</v>
-      </c>
       <c r="BC13">
         <v>3</v>
       </c>
-      <c r="BD13" t="s">
-        <v>1</v>
-      </c>
       <c r="BE13">
         <v>3</v>
       </c>
@@ -7901,24 +7678,15 @@
       <c r="BK13">
         <v>2</v>
       </c>
-      <c r="BL13" t="s">
-        <v>1</v>
-      </c>
       <c r="BM13">
         <v>1.3333333333333333</v>
       </c>
       <c r="BN13">
         <v>0.33333333333333331</v>
       </c>
-      <c r="BO13" s="9" t="s">
-        <v>1</v>
-      </c>
       <c r="BP13">
         <v>2</v>
       </c>
-      <c r="BQ13" t="s">
-        <v>1</v>
-      </c>
       <c r="BR13">
         <v>1.6666666666666667</v>
       </c>
@@ -7979,9 +7747,6 @@
       <c r="CK13">
         <v>352.14285714285717</v>
       </c>
-      <c r="CL13" t="s">
-        <v>1</v>
-      </c>
       <c r="CM13">
         <v>346.26006904487917</v>
       </c>
@@ -8018,9 +7783,6 @@
       <c r="CX13">
         <v>1.5826271186440684</v>
       </c>
-      <c r="CY13" t="s">
-        <v>1</v>
-      </c>
       <c r="CZ13">
         <v>0.67386448250186137</v>
       </c>
@@ -8057,9 +7819,6 @@
       <c r="DK13">
         <v>1.6194591134581537</v>
       </c>
-      <c r="DL13" t="s">
-        <v>1</v>
-      </c>
       <c r="DM13">
         <v>0.52249330136793104</v>
       </c>
@@ -8096,9 +7855,6 @@
       <c r="DX13">
         <v>1.8189167340339547E-2</v>
       </c>
-      <c r="DY13" t="s">
-        <v>1</v>
-      </c>
       <c r="DZ13">
         <v>0.34201321414691016</v>
       </c>
@@ -8173,9 +7929,6 @@
       </c>
       <c r="EX13">
         <v>-0.57430499679252422</v>
-      </c>
-      <c r="EY13" t="s">
-        <v>1</v>
       </c>
       <c r="EZ13">
         <v>-0.50486075342846581</v>
@@ -8213,9 +7966,6 @@
       <c r="FK13">
         <f t="shared" si="1"/>
         <v>0.39474096025859551</v>
-      </c>
-      <c r="FL13" t="s">
-        <v>1</v>
       </c>
       <c r="FM13">
         <f t="shared" si="0"/>
@@ -8995,9 +8745,6 @@
       <c r="BH15">
         <v>7</v>
       </c>
-      <c r="BI15" t="s">
-        <v>1</v>
-      </c>
       <c r="BJ15">
         <v>5.666666666666667</v>
       </c>
@@ -9034,9 +8781,6 @@
       <c r="BU15">
         <v>4.333333333333333</v>
       </c>
-      <c r="BV15" t="s">
-        <v>1</v>
-      </c>
       <c r="BW15">
         <v>3</v>
       </c>
@@ -9142,9 +8886,6 @@
       <c r="DE15">
         <v>1.0953177257525084</v>
       </c>
-      <c r="DF15" t="s">
-        <v>1</v>
-      </c>
       <c r="DG15">
         <v>3.3174075612796012</v>
       </c>
@@ -9181,9 +8922,6 @@
       <c r="DR15">
         <v>1.0057835525273333</v>
       </c>
-      <c r="DS15" t="s">
-        <v>1</v>
-      </c>
       <c r="DT15">
         <v>3.0475049900199602</v>
       </c>
@@ -9219,9 +8957,6 @@
       </c>
       <c r="EE15">
         <v>0.22838137472283809</v>
-      </c>
-      <c r="EF15" t="s">
-        <v>1</v>
       </c>
       <c r="EG15">
         <v>0.32335069444444448</v>
@@ -9526,9 +9261,6 @@
       <c r="BA16">
         <v>1</v>
       </c>
-      <c r="BB16" s="6" t="s">
-        <v>1</v>
-      </c>
       <c r="BC16">
         <v>1</v>
       </c>
@@ -9565,9 +9297,6 @@
       <c r="BN16">
         <v>1.3333333333333333</v>
       </c>
-      <c r="BO16" s="9" t="s">
-        <v>1</v>
-      </c>
       <c r="BP16">
         <v>0.33333333333333331</v>
       </c>
@@ -9688,9 +9417,6 @@
       <c r="DC16">
         <v>5.5019157088122617</v>
       </c>
-      <c r="DD16" t="s">
-        <v>1</v>
-      </c>
       <c r="DE16">
         <v>2.7362040133779262</v>
       </c>
@@ -9727,9 +9453,6 @@
       <c r="DP16">
         <v>5.0096982758620694</v>
       </c>
-      <c r="DQ16" t="s">
-        <v>1</v>
-      </c>
       <c r="DR16">
         <v>2.5003961337347484</v>
       </c>
@@ -9765,9 +9488,6 @@
       </c>
       <c r="EC16">
         <v>0.42484969939879763</v>
-      </c>
-      <c r="ED16" t="s">
-        <v>1</v>
       </c>
       <c r="EE16">
         <v>0.31263858093126384</v>
@@ -10405,9 +10125,6 @@
       <c r="FF17">
         <v>4.7100453938366038E-2</v>
       </c>
-      <c r="FG17" t="s">
-        <v>1</v>
-      </c>
       <c r="FH17">
         <v>1.2199521247385066</v>
       </c>
@@ -10452,9 +10169,6 @@
       <c r="FS17">
         <f t="shared" si="0"/>
         <v>-0.55561188937602468</v>
-      </c>
-      <c r="FT17" t="s">
-        <v>1</v>
       </c>
       <c r="FU17">
         <f t="shared" si="0"/>
@@ -10653,9 +10367,6 @@
       <c r="BI18">
         <v>3</v>
       </c>
-      <c r="BJ18" t="s">
-        <v>1</v>
-      </c>
       <c r="BK18">
         <v>0</v>
       </c>
@@ -10692,9 +10403,6 @@
       <c r="BV18">
         <v>3</v>
       </c>
-      <c r="BW18" t="s">
-        <v>1</v>
-      </c>
       <c r="BX18">
         <v>8.1835813730196829</v>
       </c>
@@ -10940,9 +10648,6 @@
       </c>
       <c r="FA18">
         <v>-1.0835563421625458</v>
-      </c>
-      <c r="FB18" t="s">
-        <v>1</v>
       </c>
       <c r="FC18">
         <v>0.39816939041716731</v>
@@ -10983,9 +10688,6 @@
       <c r="FN18">
         <f t="shared" ref="FN18:FN36" si="4">EN18-FA18</f>
         <v>-0.4472792698472039</v>
-      </c>
-      <c r="FO18" t="s">
-        <v>1</v>
       </c>
       <c r="FP18">
         <f t="shared" ref="FP18:FP37" si="5">EP18-FC18</f>
@@ -11171,9 +10873,6 @@
       <c r="AX19">
         <v>1</v>
       </c>
-      <c r="AY19" t="s">
-        <v>1</v>
-      </c>
       <c r="AZ19">
         <v>0</v>
       </c>
@@ -11189,9 +10888,6 @@
       <c r="BD19">
         <v>1</v>
       </c>
-      <c r="BE19" t="s">
-        <v>1</v>
-      </c>
       <c r="BF19">
         <v>1.6666666666666667</v>
       </c>
@@ -11204,15 +10900,9 @@
       <c r="BI19">
         <v>3</v>
       </c>
-      <c r="BJ19" t="s">
-        <v>1</v>
-      </c>
       <c r="BK19">
         <v>0.66666666666666663</v>
       </c>
-      <c r="BL19" t="s">
-        <v>1</v>
-      </c>
       <c r="BM19">
         <v>0</v>
       </c>
@@ -11242,9 +10932,6 @@
       </c>
       <c r="BV19">
         <v>0.33333333333333331</v>
-      </c>
-      <c r="BW19" t="s">
-        <v>1</v>
       </c>
       <c r="BX19">
         <v>2.3658185309649546</v>
@@ -13388,9 +13075,6 @@
       <c r="BA23">
         <v>1.6666666666666667</v>
       </c>
-      <c r="BB23" s="6" t="s">
-        <v>1</v>
-      </c>
       <c r="BC23">
         <v>2</v>
       </c>
@@ -13427,9 +13111,6 @@
       <c r="BN23">
         <v>1.3333333333333333</v>
       </c>
-      <c r="BO23" s="9" t="s">
-        <v>1</v>
-      </c>
       <c r="BP23">
         <v>3</v>
       </c>
@@ -13466,9 +13147,6 @@
       <c r="CA23">
         <v>15.429902912621358</v>
       </c>
-      <c r="CB23" t="s">
-        <v>1</v>
-      </c>
       <c r="CC23">
         <v>7.1907621247113171</v>
       </c>
@@ -13505,9 +13183,6 @@
       <c r="CN23">
         <v>341.03500761035014</v>
       </c>
-      <c r="CO23" t="s">
-        <v>1</v>
-      </c>
       <c r="CP23">
         <v>341.24694376528117</v>
       </c>
@@ -13661,9 +13336,6 @@
       <c r="EN23">
         <v>0.50389334037696309</v>
       </c>
-      <c r="EO23" t="s">
-        <v>1</v>
-      </c>
       <c r="EP23">
         <v>-0.57228052220322523</v>
       </c>
@@ -13699,9 +13371,6 @@
       </c>
       <c r="FA23">
         <v>-0.21141583638360717</v>
-      </c>
-      <c r="FB23" t="s">
-        <v>1</v>
       </c>
       <c r="FC23">
         <v>-0.94233422398725819</v>
@@ -13742,9 +13411,6 @@
       <c r="FN23">
         <f t="shared" si="4"/>
         <v>0.71530917676057026</v>
-      </c>
-      <c r="FO23" t="s">
-        <v>1</v>
       </c>
       <c r="FP23">
         <f t="shared" si="5"/>
@@ -14653,9 +14319,6 @@
       <c r="DC25">
         <v>6.314176245210728</v>
       </c>
-      <c r="DD25" t="s">
-        <v>1</v>
-      </c>
       <c r="DE25">
         <v>7.2532347504621066</v>
       </c>
@@ -14692,9 +14355,6 @@
       <c r="DP25">
         <v>5.169181034482758</v>
       </c>
-      <c r="DQ25" t="s">
-        <v>1</v>
-      </c>
       <c r="DR25">
         <v>3.7652106632904263</v>
       </c>
@@ -14730,9 +14390,6 @@
       </c>
       <c r="EC25">
         <v>1.2645290581162325</v>
-      </c>
-      <c r="ED25" t="s">
-        <v>1</v>
       </c>
       <c r="EE25">
         <v>4.5374362994903956</v>
@@ -15043,9 +14700,6 @@
       <c r="BA26">
         <v>0.33333333333333331</v>
       </c>
-      <c r="BB26" s="6" t="s">
-        <v>1</v>
-      </c>
       <c r="BC26">
         <v>5.333333333333333</v>
       </c>
@@ -15064,12 +14718,6 @@
       <c r="BH26">
         <v>8.3333333333333339</v>
       </c>
-      <c r="BI26" t="s">
-        <v>1</v>
-      </c>
-      <c r="BJ26" t="s">
-        <v>1</v>
-      </c>
       <c r="BK26">
         <v>2.3333333333333335</v>
       </c>
@@ -15082,9 +14730,6 @@
       <c r="BN26">
         <v>0.33333333333333331</v>
       </c>
-      <c r="BO26" s="9" t="s">
-        <v>1</v>
-      </c>
       <c r="BP26">
         <v>1.3333333333333333</v>
       </c>
@@ -15102,12 +14747,6 @@
       </c>
       <c r="BU26">
         <v>7.666666666666667</v>
-      </c>
-      <c r="BV26" t="s">
-        <v>1</v>
-      </c>
-      <c r="BW26" t="s">
-        <v>1</v>
       </c>
       <c r="BX26">
         <v>7.4308209313490163</v>
@@ -16702,9 +16341,6 @@
       <c r="BB29" s="6">
         <v>0.66666666666666663</v>
       </c>
-      <c r="BC29" t="s">
-        <v>1</v>
-      </c>
       <c r="BD29">
         <v>1.6666666666666667</v>
       </c>
@@ -16720,9 +16356,6 @@
       <c r="BH29">
         <v>2</v>
       </c>
-      <c r="BI29" t="s">
-        <v>1</v>
-      </c>
       <c r="BJ29">
         <v>3</v>
       </c>
@@ -16741,9 +16374,6 @@
       <c r="BO29" s="9">
         <v>0</v>
       </c>
-      <c r="BP29" t="s">
-        <v>1</v>
-      </c>
       <c r="BQ29">
         <v>1</v>
       </c>
@@ -16759,9 +16389,6 @@
       <c r="BU29">
         <v>0.33333333333333331</v>
       </c>
-      <c r="BV29" t="s">
-        <v>1</v>
-      </c>
       <c r="BW29">
         <v>2.6666666666666665</v>
       </c>
@@ -16819,9 +16446,6 @@
       <c r="CO29">
         <v>299.87577639751549</v>
       </c>
-      <c r="CP29" t="s">
-        <v>1</v>
-      </c>
       <c r="CQ29">
         <v>352.20297029702976</v>
       </c>
@@ -17013,9 +16637,6 @@
       </c>
       <c r="FB29">
         <v>-3.5370908592812067</v>
-      </c>
-      <c r="FC29" t="s">
-        <v>1</v>
       </c>
       <c r="FD29">
         <v>0.38108043419757404</v>
@@ -17057,9 +16678,6 @@
       <c r="FO29">
         <f t="shared" si="13"/>
         <v>3.3063563181321851</v>
-      </c>
-      <c r="FP29" t="s">
-        <v>1</v>
       </c>
       <c r="FQ29">
         <f t="shared" si="6"/>
@@ -17250,9 +16868,6 @@
       <c r="BA30">
         <v>1</v>
       </c>
-      <c r="BB30" s="6" t="s">
-        <v>1</v>
-      </c>
       <c r="BC30">
         <v>1</v>
       </c>
@@ -17265,18 +16880,12 @@
       <c r="BF30">
         <v>4.666666666666667</v>
       </c>
-      <c r="BG30" t="s">
-        <v>1</v>
-      </c>
       <c r="BH30">
         <v>6.666666666666667</v>
       </c>
       <c r="BI30">
         <v>12</v>
       </c>
-      <c r="BJ30" t="s">
-        <v>1</v>
-      </c>
       <c r="BK30">
         <v>2.6666666666666665</v>
       </c>
@@ -17289,9 +16898,6 @@
       <c r="BN30">
         <v>1</v>
       </c>
-      <c r="BO30" s="9" t="s">
-        <v>1</v>
-      </c>
       <c r="BP30">
         <v>0.66666666666666663</v>
       </c>
@@ -17304,18 +16910,12 @@
       <c r="BS30">
         <v>3.3333333333333335</v>
       </c>
-      <c r="BT30" t="s">
-        <v>1</v>
-      </c>
       <c r="BU30">
         <v>2.3333333333333335</v>
       </c>
       <c r="BV30">
         <v>8</v>
       </c>
-      <c r="BW30" t="s">
-        <v>1</v>
-      </c>
       <c r="BX30">
         <v>2.935765722515602</v>
       </c>
@@ -17430,9 +17030,6 @@
       <c r="DI30">
         <v>8.971134020618555</v>
       </c>
-      <c r="DJ30" t="s">
-        <v>1</v>
-      </c>
       <c r="DK30">
         <v>1.8406945111217798</v>
       </c>
@@ -17469,9 +17066,6 @@
       <c r="DV30">
         <v>4.293516699410608</v>
       </c>
-      <c r="DW30" t="s">
-        <v>1</v>
-      </c>
       <c r="DX30">
         <v>-6.6693613581244884E-2</v>
       </c>
@@ -17508,9 +17102,6 @@
       <c r="EI30">
         <v>6.1575918548030106</v>
       </c>
-      <c r="EJ30" t="s">
-        <v>1</v>
-      </c>
       <c r="EK30">
         <v>-0.58467578301494838</v>
       </c>
@@ -17585,9 +17176,6 @@
       </c>
       <c r="FI30">
         <v>0.15744500097114447</v>
-      </c>
-      <c r="FJ30" t="s">
-        <v>1</v>
       </c>
       <c r="FK30">
         <f t="shared" si="1"/>
@@ -17636,9 +17224,6 @@
       <c r="FV30">
         <f t="shared" si="11"/>
         <v>-0.47700819304913467</v>
-      </c>
-      <c r="FW30" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:179" x14ac:dyDescent="0.35">
@@ -18470,9 +18055,6 @@
       <c r="CN32">
         <v>336.3774733637747</v>
       </c>
-      <c r="CO32" t="s">
-        <v>1</v>
-      </c>
       <c r="CP32">
         <v>345.4034229828851</v>
       </c>
@@ -18664,9 +18246,6 @@
       </c>
       <c r="FA32">
         <v>-0.56820058874772328</v>
-      </c>
-      <c r="FB32" t="s">
-        <v>1</v>
       </c>
       <c r="FC32">
         <v>-0.38379105131874824</v>
@@ -18707,9 +18286,6 @@
       <c r="FN32">
         <f t="shared" si="4"/>
         <v>0.29243143335033855</v>
-      </c>
-      <c r="FO32" t="s">
-        <v>1</v>
       </c>
       <c r="FP32">
         <f t="shared" si="5"/>
@@ -18901,12 +18477,6 @@
       <c r="AZ33">
         <v>1</v>
       </c>
-      <c r="BA33" t="s">
-        <v>1</v>
-      </c>
-      <c r="BB33" s="6" t="s">
-        <v>1</v>
-      </c>
       <c r="BC33">
         <v>2.3333333333333335</v>
       </c>
@@ -18943,9 +18513,6 @@
       <c r="BN33">
         <v>0</v>
       </c>
-      <c r="BO33" s="9" t="s">
-        <v>1</v>
-      </c>
       <c r="BP33">
         <v>2</v>
       </c>
@@ -19021,9 +18588,6 @@
       <c r="CN33">
         <v>334.82496194824961</v>
       </c>
-      <c r="CO33" t="s">
-        <v>1</v>
-      </c>
       <c r="CP33">
         <v>345.4034229828851</v>
       </c>
@@ -19215,9 +18779,6 @@
       </c>
       <c r="FA33">
         <v>-0.68712883953575754</v>
-      </c>
-      <c r="FB33" t="s">
-        <v>1</v>
       </c>
       <c r="FC33">
         <v>-0.38379105131874824</v>
@@ -19258,9 +18819,6 @@
       <c r="FN33">
         <f t="shared" si="4"/>
         <v>-0.52280909890833005</v>
-      </c>
-      <c r="FO33" t="s">
-        <v>1</v>
       </c>
       <c r="FP33">
         <f t="shared" si="5"/>
@@ -19410,9 +18968,6 @@
       <c r="AL34">
         <v>70.951669157947194</v>
       </c>
-      <c r="AM34" t="s">
-        <v>1</v>
-      </c>
       <c r="AN34">
         <v>79.725645198790957</v>
       </c>
@@ -21066,12 +20621,6 @@
       <c r="AL37">
         <v>0</v>
       </c>
-      <c r="AM37" t="s">
-        <v>1</v>
-      </c>
-      <c r="AN37" t="s">
-        <v>1</v>
-      </c>
       <c r="AO37">
         <v>63.801728060000002</v>
       </c>
@@ -21096,21 +20645,9 @@
       <c r="AV37">
         <v>42.008733624454145</v>
       </c>
-      <c r="AW37" t="s">
-        <v>1</v>
-      </c>
       <c r="AX37">
         <v>3</v>
       </c>
-      <c r="AY37" t="s">
-        <v>1</v>
-      </c>
-      <c r="AZ37" t="s">
-        <v>1</v>
-      </c>
-      <c r="BA37" t="s">
-        <v>1</v>
-      </c>
       <c r="BB37" s="6">
         <v>1</v>
       </c>
@@ -21126,30 +20663,15 @@
       <c r="BF37">
         <v>8.3333333333333339</v>
       </c>
-      <c r="BG37" t="s">
-        <v>1</v>
-      </c>
       <c r="BH37">
         <v>2</v>
       </c>
       <c r="BI37">
         <v>2.3333333333333335</v>
       </c>
-      <c r="BJ37" t="s">
-        <v>1</v>
-      </c>
       <c r="BK37">
         <v>3.6666666666666665</v>
       </c>
-      <c r="BL37" t="s">
-        <v>1</v>
-      </c>
-      <c r="BM37" t="s">
-        <v>1</v>
-      </c>
-      <c r="BN37" t="s">
-        <v>1</v>
-      </c>
       <c r="BO37" s="9">
         <v>0.33333333333333331</v>
       </c>
@@ -21165,30 +20687,18 @@
       <c r="BS37">
         <v>2.3333333333333335</v>
       </c>
-      <c r="BT37" t="s">
-        <v>1</v>
-      </c>
       <c r="BU37">
         <v>0.33333333333333331</v>
       </c>
       <c r="BV37">
         <v>1.3333333333333333</v>
       </c>
-      <c r="BW37" t="s">
-        <v>1</v>
-      </c>
       <c r="BX37">
         <v>2.8247557003257331</v>
       </c>
       <c r="BY37">
         <v>10.491593274619696</v>
       </c>
-      <c r="BZ37" t="s">
-        <v>1</v>
-      </c>
-      <c r="CA37" t="s">
-        <v>1</v>
-      </c>
       <c r="CB37">
         <v>22.260201632261165</v>
       </c>
@@ -21201,9 +20711,6 @@
       <c r="CE37">
         <v>6.8855505279034688</v>
       </c>
-      <c r="CF37" t="s">
-        <v>1</v>
-      </c>
       <c r="CG37">
         <v>13.229484029484027</v>
       </c>
@@ -21222,12 +20729,6 @@
       <c r="CL37">
         <v>336.86996547756041</v>
       </c>
-      <c r="CM37" t="s">
-        <v>1</v>
-      </c>
-      <c r="CN37" t="s">
-        <v>1</v>
-      </c>
       <c r="CO37">
         <v>348.9751552795031</v>
       </c>
@@ -21252,21 +20753,12 @@
       <c r="CV37">
         <v>345.54896142433239</v>
       </c>
-      <c r="CW37" t="s">
-        <v>1</v>
-      </c>
       <c r="CX37">
         <v>2.0254237288135597</v>
       </c>
       <c r="CY37">
         <v>3.0640357408786296</v>
       </c>
-      <c r="CZ37" t="s">
-        <v>1</v>
-      </c>
-      <c r="DA37" t="s">
-        <v>1</v>
-      </c>
       <c r="DB37">
         <v>4.0014903129657222</v>
       </c>
@@ -21279,9 +20771,6 @@
       <c r="DE37">
         <v>2.3752310536044363</v>
       </c>
-      <c r="DF37" t="s">
-        <v>1</v>
-      </c>
       <c r="DG37">
         <v>7.7752388865808051</v>
       </c>
@@ -21291,21 +20780,12 @@
       <c r="DI37">
         <v>5.2226804123711332</v>
       </c>
-      <c r="DJ37" t="s">
-        <v>1</v>
-      </c>
       <c r="DK37">
         <v>2.1127380380860941</v>
       </c>
       <c r="DL37">
         <v>1.032999576928501</v>
       </c>
-      <c r="DM37" t="s">
-        <v>1</v>
-      </c>
-      <c r="DN37" t="s">
-        <v>1</v>
-      </c>
       <c r="DO37">
         <v>2.9962373988357234</v>
       </c>
@@ -21318,9 +20798,6 @@
       <c r="DR37">
         <v>1.6751072659492161</v>
       </c>
-      <c r="DS37" t="s">
-        <v>1</v>
-      </c>
       <c r="DT37">
         <v>2.4063872255489014</v>
       </c>
@@ -21330,21 +20807,12 @@
       <c r="DV37">
         <v>2.849901768172888</v>
       </c>
-      <c r="DW37" t="s">
-        <v>1</v>
-      </c>
       <c r="DX37">
         <v>-7.6798706548100185E-2</v>
       </c>
       <c r="DY37">
         <v>2.7574815390594636</v>
       </c>
-      <c r="DZ37" t="s">
-        <v>1</v>
-      </c>
-      <c r="EA37" t="s">
-        <v>1</v>
-      </c>
       <c r="EB37">
         <v>1.28515625</v>
       </c>
@@ -21357,9 +20825,6 @@
       <c r="EE37">
         <v>0.98392787142297133</v>
       </c>
-      <c r="EF37" t="s">
-        <v>1</v>
-      </c>
       <c r="EG37">
         <v>7.0160590277777768</v>
       </c>
@@ -21369,21 +20834,12 @@
       <c r="EI37">
         <v>3.1606905710491366</v>
       </c>
-      <c r="EJ37" t="s">
-        <v>1</v>
-      </c>
       <c r="EK37">
         <v>-0.63898675207899436</v>
       </c>
       <c r="EL37">
         <v>0.90662694298667734</v>
       </c>
-      <c r="EM37" t="s">
-        <v>1</v>
-      </c>
-      <c r="EN37" t="s">
-        <v>1</v>
-      </c>
       <c r="EO37">
         <v>1.1158396380009423</v>
       </c>
@@ -21396,9 +20852,6 @@
       <c r="ER37">
         <v>-0.32853478421207982</v>
       </c>
-      <c r="ES37" t="s">
-        <v>1</v>
-      </c>
       <c r="ET37">
         <v>5.3527215208639775E-2</v>
       </c>
@@ -21417,12 +20870,6 @@
       <c r="EY37">
         <v>-0.21435727106771249</v>
       </c>
-      <c r="EZ37" t="s">
-        <v>1</v>
-      </c>
-      <c r="FA37" t="s">
-        <v>1</v>
-      </c>
       <c r="FB37">
         <v>0.23764912165584226</v>
       </c>
@@ -21446,9 +20893,6 @@
       </c>
       <c r="FI37">
         <v>8.6704823703250847E-2</v>
-      </c>
-      <c r="FJ37" t="s">
-        <v>1</v>
       </c>
       <c r="FK37">
         <f t="shared" si="1"/>
@@ -21458,12 +20902,6 @@
         <f t="shared" si="2"/>
         <v>1.1209842140543897</v>
       </c>
-      <c r="FM37" t="s">
-        <v>1</v>
-      </c>
-      <c r="FN37" t="s">
-        <v>1</v>
-      </c>
       <c r="FO37">
         <f t="shared" si="13"/>
         <v>0.87819051634510004</v>
@@ -21480,9 +20918,6 @@
         <f t="shared" si="7"/>
         <v>-0.17839540483955432</v>
       </c>
-      <c r="FS37" t="s">
-        <v>1</v>
-      </c>
       <c r="FT37">
         <f t="shared" si="9"/>
         <v>-6.2868107175499482E-2</v>
@@ -21494,9 +20929,6 @@
       <c r="FV37">
         <f t="shared" si="11"/>
         <v>-1.1350963485906915</v>
-      </c>
-      <c r="FW37" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made new graphs and updated readme
</commit_message>
<xml_diff>
--- a/GreenIguanaMasterSpring2021.xlsx
+++ b/GreenIguanaMasterSpring2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usu-my.sharepoint.com/personal/a02308724_aggies_usu_edu/Documents/Desktop/ASU green iguana 2021/greeniguanaAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="298" documentId="8_{D3E1F204-3744-4711-9BBE-5D795E9D066E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39028A04-6B9F-4AD6-AE7C-C013F351694F}"/>
+  <xr:revisionPtr revIDLastSave="300" documentId="8_{D3E1F204-3744-4711-9BBE-5D795E9D066E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86DEEA17-38A6-485D-9282-C1551794D1E9}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1470" windowWidth="25440" windowHeight="15390" xr2:uid="{480D2B5B-0BF7-4EFB-BBDF-5EF1CCA213B8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{480D2B5B-0BF7-4EFB-BBDF-5EF1CCA213B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Assay" sheetId="2" r:id="rId1"/>
@@ -35,12 +35,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="225">
   <si>
     <t>0324bka</t>
-  </si>
-  <si>
-    <t>na</t>
   </si>
   <si>
     <t>0423bka</t>
@@ -1109,8 +1106,8 @@
   <dimension ref="A1:FY37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F15" sqref="F15"/>
+      <pane xSplit="1" topLeftCell="BH1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BO9" sqref="BO9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1123,547 +1120,547 @@
   <sheetData>
     <row r="1" spans="1:181" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AR1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AS1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AT1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AU1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AV1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AW1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AX1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AY1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AZ1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="BA1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="BB1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="BC1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="BD1" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="BE1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="BF1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="BG1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="BH1" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="BI1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="BJ1" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="BK1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="BL1" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="BM1" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="BN1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="BO1" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="BP1" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="BQ1" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="BR1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="BS1" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="BT1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="BU1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="BV1" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="BW1" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="BX1" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="BY1" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="BZ1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="CA1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="CB1" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="CC1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="CD1" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="CE1" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="CF1" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="CG1" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="CH1" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="CI1" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="CJ1" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="CK1" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="CL1" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="CM1" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="CN1" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="CO1" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="CP1" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="CQ1" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="CR1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="CS1" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="CT1" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="CU1" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="CV1" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="CW1" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="CX1" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="CY1" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="CZ1" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="DA1" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="DB1" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="DC1" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="DD1" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="DE1" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="DF1" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="DG1" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="DH1" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="DI1" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="DJ1" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="DK1" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="DL1" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="DM1" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="DN1" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="DO1" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="DP1" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="DQ1" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="DR1" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="DS1" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="DT1" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="DU1" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="DV1" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="DW1" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="DX1" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="DY1" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="DZ1" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="EA1" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="EB1" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="EC1" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="ED1" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="EE1" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="EF1" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="EG1" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="EH1" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="EI1" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="EJ1" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="EK1" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="EL1" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="EM1" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AD1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AG1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AH1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AI1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AJ1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AL1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="AM1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AN1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AO1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="AP1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="AQ1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="AR1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AS1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="AT1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AU1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AV1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="AW1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AX1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="AY1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="AZ1" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="BA1" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="BB1" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="BC1" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="BD1" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="BE1" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="BF1" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="BG1" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="BH1" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="BI1" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="BJ1" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="BK1" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="BL1" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="BM1" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="BN1" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="BO1" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="BP1" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="BQ1" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="BR1" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="BS1" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="BT1" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="BU1" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="BV1" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="BW1" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="BX1" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="BY1" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="BZ1" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="CA1" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="CB1" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="CC1" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="CD1" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="CE1" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="CF1" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="CG1" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="CH1" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="CI1" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="CJ1" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="CK1" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="CL1" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="CM1" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="CN1" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="CO1" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="CP1" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="CQ1" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="CR1" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="CS1" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="CT1" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="CU1" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="CV1" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="CW1" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="CX1" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="CY1" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="CZ1" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="DA1" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="DB1" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="DC1" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="DD1" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="DE1" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="DF1" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="DG1" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="DH1" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="DI1" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="DJ1" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="DK1" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="DL1" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="DM1" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="DN1" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="DO1" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="DP1" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="DQ1" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="DR1" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="DS1" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="DT1" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="DU1" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="DV1" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="DW1" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="DX1" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="DY1" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="DZ1" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="EA1" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="EB1" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="EC1" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="ED1" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="EE1" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="EF1" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="EG1" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="EH1" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="EI1" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="EJ1" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="EK1" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="EL1" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="EM1" s="3" t="s">
+      <c r="EN1" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="EN1" s="3" t="s">
+      <c r="EO1" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="EO1" s="3" t="s">
+      <c r="EP1" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="EP1" s="3" t="s">
+      <c r="EQ1" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="EQ1" s="3" t="s">
+      <c r="ER1" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="ER1" s="3" t="s">
+      <c r="ES1" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="ES1" s="3" t="s">
+      <c r="ET1" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="ET1" s="3" t="s">
+      <c r="EU1" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="EU1" s="3" t="s">
+      <c r="EV1" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="EV1" s="3" t="s">
+      <c r="EW1" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="EW1" s="3" t="s">
+      <c r="EX1" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="EX1" s="3" t="s">
+      <c r="EY1" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="EY1" s="3" t="s">
+      <c r="EZ1" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="EZ1" s="3" t="s">
+      <c r="FA1" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="FA1" s="3" t="s">
+      <c r="FB1" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="FB1" s="3" t="s">
+      <c r="FC1" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="FC1" s="3" t="s">
+      <c r="FD1" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="FD1" s="3" t="s">
+      <c r="FE1" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="FE1" s="3" t="s">
+      <c r="FF1" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="FF1" s="3" t="s">
+      <c r="FG1" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="FG1" s="3" t="s">
+      <c r="FH1" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="FH1" s="3" t="s">
+      <c r="FI1" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="FI1" s="3" t="s">
+      <c r="FJ1" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="FJ1" s="3" t="s">
+      <c r="FK1" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="FK1" s="3" t="s">
+      <c r="FL1" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="FL1" s="3" t="s">
+      <c r="FM1" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="FM1" s="3" t="s">
+      <c r="FN1" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="FN1" s="3" t="s">
+      <c r="FO1" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="FO1" s="3" t="s">
+      <c r="FP1" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="FP1" s="3" t="s">
+      <c r="FQ1" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="FQ1" s="3" t="s">
+      <c r="FR1" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="FR1" s="3" t="s">
+      <c r="FS1" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="FS1" s="3" t="s">
+      <c r="FT1" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="FT1" s="3" t="s">
+      <c r="FU1" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="FU1" s="3" t="s">
+      <c r="FV1" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="FV1" s="3" t="s">
+      <c r="FW1" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="FW1" s="3" t="s">
+      <c r="FX1" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="FX1" s="3" t="s">
+      <c r="FY1" s="3" t="s">
         <v>217</v>
-      </c>
-      <c r="FY1" s="3" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:181" x14ac:dyDescent="0.35">
@@ -1671,19 +1668,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
         <v>49</v>
       </c>
-      <c r="C2" t="s">
-        <v>50</v>
-      </c>
       <c r="D2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -2192,19 +2189,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
         <v>52</v>
       </c>
-      <c r="C3" t="s">
-        <v>53</v>
-      </c>
       <c r="D3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -2747,19 +2744,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s">
         <v>49</v>
       </c>
-      <c r="C4" t="s">
-        <v>50</v>
-      </c>
       <c r="D4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -3287,19 +3284,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -3833,19 +3830,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
         <v>52</v>
       </c>
-      <c r="C6" t="s">
-        <v>53</v>
-      </c>
       <c r="D6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -4366,19 +4363,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -4556,9 +4553,6 @@
       </c>
       <c r="BO7">
         <v>0.66666666666666663</v>
-      </c>
-      <c r="BP7" t="s">
-        <v>1</v>
       </c>
       <c r="BQ7" s="9">
         <v>0</v>
@@ -4918,19 +4912,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
         <v>49</v>
       </c>
-      <c r="C8" t="s">
-        <v>50</v>
-      </c>
       <c r="D8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -5457,19 +5451,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -6012,19 +6006,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -6157,9 +6151,6 @@
       </c>
       <c r="BA10">
         <v>2</v>
-      </c>
-      <c r="BB10" t="s">
-        <v>1</v>
       </c>
       <c r="BC10">
         <v>0</v>
@@ -6518,19 +6509,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E11" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -7016,19 +7007,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -7566,19 +7557,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -8084,19 +8075,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -8642,19 +8633,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -9182,19 +9173,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -9722,19 +9713,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -10270,19 +10261,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D18" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -10812,19 +10803,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -11352,19 +11343,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -11907,19 +11898,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D21" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E21" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F21" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -12462,19 +12453,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F22" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -13020,19 +13011,19 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F23" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -13556,19 +13547,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E24" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F24" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -14111,19 +14102,19 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E25" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F25" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G25">
         <v>0</v>
@@ -14657,19 +14648,19 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E26" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G26">
         <v>0</v>
@@ -15194,19 +15185,19 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D27" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E27" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F27" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -15749,19 +15740,19 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D28" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E28" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F28" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G28">
         <v>0</v>
@@ -16304,19 +16295,19 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E29" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F29" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G29">
         <v>1</v>
@@ -16840,19 +16831,19 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E30" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -17361,19 +17352,19 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D31" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E31" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F31" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -17916,19 +17907,19 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E32" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F32" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -18461,19 +18452,19 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D33" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E33" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F33" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -18997,19 +18988,19 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E34" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F34" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G34">
         <v>0</v>
@@ -19549,19 +19540,19 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D35" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E35" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F35" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G35">
         <v>0</v>
@@ -20104,19 +20095,19 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D36" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E36" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F36" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -20659,19 +20650,19 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C37" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D37" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E37" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F37" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G37">
         <v>0</v>
@@ -21109,164 +21100,164 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
         <v>61</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>62</v>
-      </c>
-      <c r="C4" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" s="4">
         <v>44279</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6" s="4">
         <v>44309</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" s="4">
         <v>44314</v>
       </c>
       <c r="C7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B8" s="4">
         <v>44316</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B9" s="4">
         <v>44320</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B10" s="4">
         <v>44327</v>
       </c>
       <c r="C10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B11" s="4">
         <v>44341</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B12" s="4">
         <v>44344</v>
       </c>
       <c r="C12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B13" s="4">
         <v>44346</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B14" s="4">
         <v>44350</v>
       </c>
       <c r="C14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B15" s="4">
         <v>44357</v>
       </c>
       <c r="C15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B16" s="4">
         <v>44371</v>
       </c>
       <c r="C16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B17" s="4">
         <v>44375</v>
       </c>
       <c r="C17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
deleted a bunch of stuff
</commit_message>
<xml_diff>
--- a/GreenIguanaMasterSpring2021.xlsx
+++ b/GreenIguanaMasterSpring2021.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usu-my.sharepoint.com/personal/a02308724_aggies_usu_edu/Documents/Desktop/ASU green iguana 2021/greeniguanaAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="302" documentId="8_{D3E1F204-3744-4711-9BBE-5D795E9D066E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{675627B5-2511-4514-BE69-913D751D5CE8}"/>
+  <xr:revisionPtr revIDLastSave="327" documentId="8_{D3E1F204-3744-4711-9BBE-5D795E9D066E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E4FDF20-11AA-4EC8-A31B-A2576A961C42}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-1470" windowWidth="25440" windowHeight="15390" xr2:uid="{480D2B5B-0BF7-4EFB-BBDF-5EF1CCA213B8}"/>
   </bookViews>
@@ -778,7 +778,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -789,6 +789,8 @@
     <xf numFmtId="16" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1106,8 +1108,8 @@
   <dimension ref="A1:FY37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="FM1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="FT12" sqref="FT12"/>
+      <pane xSplit="1" topLeftCell="EN1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="ER19" sqref="ER19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1115,6 +1117,7 @@
     <col min="1" max="1" width="9.6328125" style="3"/>
     <col min="56" max="56" width="9.6328125" style="6"/>
     <col min="69" max="69" width="9.6328125" style="9"/>
+    <col min="130" max="130" width="9.6328125" style="11"/>
     <col min="167" max="167" width="9.6328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1506,7 +1509,7 @@
       <c r="DY1" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="DZ1" s="3" t="s">
+      <c r="DZ1" s="10" t="s">
         <v>164</v>
       </c>
       <c r="EA1" s="3" t="s">
@@ -2024,7 +2027,7 @@
       <c r="DY2">
         <v>2.7308447937131626</v>
       </c>
-      <c r="DZ2">
+      <c r="DZ2" s="11">
         <v>0.18997574777687959</v>
       </c>
       <c r="EA2">
@@ -2557,7 +2560,7 @@
       <c r="DY3">
         <v>2.7834970530451866</v>
       </c>
-      <c r="DZ3">
+      <c r="DZ3" s="11">
         <v>0.21220695230396128</v>
       </c>
       <c r="EA3">
@@ -3620,8 +3623,8 @@
       <c r="DY5">
         <v>5.4805500982318254</v>
       </c>
-      <c r="DZ5">
-        <v>-9.7008892481810799E-2</v>
+      <c r="DZ5" s="11">
+        <v>0</v>
       </c>
       <c r="EA5">
         <v>5.0525464834276515E-2</v>
@@ -4147,7 +4150,7 @@
       <c r="DY6">
         <v>3.1622789783889975</v>
       </c>
-      <c r="DZ6">
+      <c r="DZ6" s="11">
         <v>1.2126111560226364E-2</v>
       </c>
       <c r="EA6">
@@ -4674,11 +4677,11 @@
       <c r="DY7">
         <v>2.0636542239685656</v>
       </c>
-      <c r="DZ7">
+      <c r="DZ7" s="11">
         <v>7.6798706548100296E-2</v>
       </c>
       <c r="EA7">
-        <v>-6.2651576394502764E-2</v>
+        <v>0</v>
       </c>
       <c r="EB7">
         <v>6.8013991449669603E-2</v>
@@ -5207,11 +5210,11 @@
       <c r="DY8">
         <v>2.4188605108055001</v>
       </c>
-      <c r="DZ8">
+      <c r="DZ8" s="11">
         <v>0.48908649959579636</v>
       </c>
       <c r="EA8">
-        <v>-3.4357316087307917E-2</v>
+        <v>0</v>
       </c>
       <c r="EB8">
         <v>0.17877963466770302</v>
@@ -5743,8 +5746,8 @@
       <c r="DY9">
         <v>5.3512770137524557</v>
       </c>
-      <c r="DZ9">
-        <v>-7.4777687954729138E-2</v>
+      <c r="DZ9" s="11">
+        <v>0</v>
       </c>
       <c r="EA9">
         <v>0.48504446240905419</v>
@@ -7257,7 +7260,7 @@
       <c r="DY12">
         <v>2.7218074656188609</v>
       </c>
-      <c r="DZ12">
+      <c r="DZ12" s="11">
         <v>9.9029911075181859E-2</v>
       </c>
       <c r="EA12">
@@ -7772,7 +7775,7 @@
       <c r="DY13">
         <v>0.79921414538310365</v>
       </c>
-      <c r="DZ13">
+      <c r="DZ13" s="11">
         <v>1.8189167340339547E-2</v>
       </c>
       <c r="EB13">
@@ -8308,8 +8311,8 @@
       <c r="DY14">
         <v>5.0255402750491154</v>
       </c>
-      <c r="DZ14">
-        <v>-4.8504446240905344E-2</v>
+      <c r="DZ14" s="11">
+        <v>0</v>
       </c>
       <c r="EA14">
         <v>0.23319082782743877</v>
@@ -8838,8 +8841,8 @@
       <c r="DY15">
         <v>3.6168958742632604</v>
       </c>
-      <c r="DZ15">
-        <v>-1.8189167340339547E-2</v>
+      <c r="DZ15" s="11">
+        <v>0</v>
       </c>
       <c r="EA15">
         <v>0.22930431403031482</v>
@@ -9365,8 +9368,8 @@
       <c r="DY16">
         <v>5.9056974459724945</v>
       </c>
-      <c r="DZ16">
-        <v>-0.10105092966855292</v>
+      <c r="DZ16" s="11">
+        <v>0</v>
       </c>
       <c r="EA16">
         <v>5.3808783521181507</v>
@@ -9904,8 +9907,8 @@
       <c r="DY17">
         <v>4.1520628683693515</v>
       </c>
-      <c r="DZ17">
-        <v>-0.10105092966855292</v>
+      <c r="DZ17" s="11">
+        <v>0</v>
       </c>
       <c r="EA17">
         <v>0.22347454333462882</v>
@@ -10434,8 +10437,8 @@
       <c r="DY18">
         <v>2.6730844793713153</v>
       </c>
-      <c r="DZ18">
-        <v>-1.6168148746968373E-2</v>
+      <c r="DZ18" s="11">
+        <v>0</v>
       </c>
       <c r="EA18">
         <v>0.32258064516129031</v>
@@ -10955,7 +10958,7 @@
       <c r="DY19">
         <v>1.3536345776031433</v>
       </c>
-      <c r="DZ19">
+      <c r="DZ19" s="11">
         <v>0.40824575586095391</v>
       </c>
       <c r="EA19">
@@ -11497,8 +11500,8 @@
       <c r="DY20">
         <v>2.5302058161819847</v>
       </c>
-      <c r="DZ20">
-        <v>-4.2441390460792164E-2</v>
+      <c r="DZ20" s="11">
+        <v>0</v>
       </c>
       <c r="EA20">
         <v>0.13408472600077731</v>
@@ -12039,7 +12042,7 @@
       <c r="DY21">
         <v>1.5061244896258645</v>
       </c>
-      <c r="DZ21">
+      <c r="DZ21" s="11">
         <v>0.28900565885206142</v>
       </c>
       <c r="EA21">
@@ -12584,8 +12587,8 @@
       <c r="DY22">
         <v>1.2632280643279725</v>
       </c>
-      <c r="DZ22">
-        <v>-0.1071139854486661</v>
+      <c r="DZ22" s="11">
+        <v>0</v>
       </c>
       <c r="EA22">
         <v>0.22347454333462882</v>
@@ -13114,7 +13117,7 @@
       <c r="DY23">
         <v>3.336805266227814</v>
       </c>
-      <c r="DZ23">
+      <c r="DZ23" s="11">
         <v>5.4567502021018635E-2</v>
       </c>
       <c r="EA23">
@@ -13650,8 +13653,8 @@
       <c r="DY24">
         <v>3.5280393300558286</v>
       </c>
-      <c r="DZ24">
-        <v>-8.8924818108326559E-2</v>
+      <c r="DZ24" s="11">
+        <v>0</v>
       </c>
       <c r="EA24">
         <v>0.34395647104547222</v>
@@ -14186,8 +14189,8 @@
       <c r="DY25">
         <v>3.1914007166069496</v>
       </c>
-      <c r="DZ25">
-        <v>-0.13540824575586094</v>
+      <c r="DZ25" s="11">
+        <v>0</v>
       </c>
       <c r="EA25">
         <v>3.0275942479595801</v>
@@ -14707,7 +14710,7 @@
       <c r="DY26">
         <v>2.2485626197816848</v>
       </c>
-      <c r="DZ26">
+      <c r="DZ26" s="11">
         <v>0.36176232821341947</v>
       </c>
       <c r="EA26">
@@ -15249,7 +15252,7 @@
       <c r="DY27">
         <v>3.0547454378801762</v>
       </c>
-      <c r="DZ27">
+      <c r="DZ27" s="11">
         <v>4.0420371867421208E-2</v>
       </c>
       <c r="EA27">
@@ -15791,8 +15794,8 @@
       <c r="DY28">
         <v>2.4539621698191816</v>
       </c>
-      <c r="DZ28">
-        <v>-8.4882780921584439E-2</v>
+      <c r="DZ28" s="11">
+        <v>0</v>
       </c>
       <c r="EA28">
         <v>0.84531675087446567</v>
@@ -16321,8 +16324,8 @@
       <c r="DY29">
         <v>6.0824097991834014</v>
       </c>
-      <c r="DZ29">
-        <v>-3.6378334680678977E-2</v>
+      <c r="DZ29" s="11">
+        <v>0</v>
       </c>
       <c r="EA29">
         <v>3.289933929265449</v>
@@ -16833,8 +16836,8 @@
       <c r="DX30">
         <v>4.293516699410608</v>
       </c>
-      <c r="DZ30">
-        <v>-6.6693613581244884E-2</v>
+      <c r="DZ30" s="11">
+        <v>0</v>
       </c>
       <c r="EA30">
         <v>1.6906335017489316</v>
@@ -17366,8 +17369,8 @@
       <c r="DY31">
         <v>2.0989917506874427</v>
       </c>
-      <c r="DZ31">
-        <v>-7.0735650767987004E-2</v>
+      <c r="DZ31" s="11">
+        <v>0</v>
       </c>
       <c r="EA31">
         <v>0.42168674698795178</v>
@@ -17905,8 +17908,8 @@
       <c r="DY32">
         <v>4.1992333972168998</v>
       </c>
-      <c r="DZ32">
-        <v>-5.6588520614389584E-2</v>
+      <c r="DZ32" s="11">
+        <v>0</v>
       </c>
       <c r="EA32">
         <v>1.4613291877186163</v>
@@ -18429,8 +18432,8 @@
       <c r="DY33">
         <v>2.5177068577618531</v>
       </c>
-      <c r="DZ33">
-        <v>-0.1071139854486661</v>
+      <c r="DZ33" s="11">
+        <v>0</v>
       </c>
       <c r="EA33">
         <v>0.16323357947920708</v>
@@ -18962,8 +18965,8 @@
       <c r="DY34">
         <v>1.4423798016831932</v>
       </c>
-      <c r="DZ34">
-        <v>-0.12530315278900558</v>
+      <c r="DZ34" s="11">
+        <v>0</v>
       </c>
       <c r="EA34">
         <v>0.60240963855421681</v>
@@ -19504,8 +19507,8 @@
       <c r="DY35">
         <v>3.4088825931172413</v>
       </c>
-      <c r="DZ35">
-        <v>-0.13338722716248991</v>
+      <c r="DZ35" s="11">
+        <v>0</v>
       </c>
       <c r="EA35">
         <v>6.607073455110761E-2</v>
@@ -20046,8 +20049,8 @@
       <c r="DY36">
         <v>3.1309890842429793</v>
       </c>
-      <c r="DZ36">
-        <v>-0.12126111560226353</v>
+      <c r="DZ36" s="11">
+        <v>0</v>
       </c>
       <c r="EA36">
         <v>0.75204041974349001</v>
@@ -20507,8 +20510,8 @@
       <c r="DX37">
         <v>2.849901768172888</v>
       </c>
-      <c r="DZ37">
-        <v>-7.6798706548100185E-2</v>
+      <c r="DZ37" s="11">
+        <v>0</v>
       </c>
       <c r="EA37">
         <v>2.7574815390594636</v>

</xml_diff>

<commit_message>
ne wlong data tri gly glu and new script
</commit_message>
<xml_diff>
--- a/GreenIguanaMasterSpring2021.xlsx
+++ b/GreenIguanaMasterSpring2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usu-my.sharepoint.com/personal/a02308724_aggies_usu_edu/Documents/Desktop/ASU green iguana 2021/greeniguanaAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="327" documentId="8_{D3E1F204-3744-4711-9BBE-5D795E9D066E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E4FDF20-11AA-4EC8-A31B-A2576A961C42}"/>
+  <xr:revisionPtr revIDLastSave="329" documentId="8_{D3E1F204-3744-4711-9BBE-5D795E9D066E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B59690EE-2B02-4788-8E1E-52D07A6B640B}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1470" windowWidth="25440" windowHeight="15390" xr2:uid="{480D2B5B-0BF7-4EFB-BBDF-5EF1CCA213B8}"/>
+    <workbookView xWindow="-19310" yWindow="-470" windowWidth="19420" windowHeight="10420" xr2:uid="{480D2B5B-0BF7-4EFB-BBDF-5EF1CCA213B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Assay" sheetId="2" r:id="rId1"/>
@@ -1108,20 +1108,21 @@
   <dimension ref="A1:FY37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="EN1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="ER19" sqref="ER19"/>
+      <pane xSplit="1" topLeftCell="CV1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6328125" style="3"/>
-    <col min="56" max="56" width="9.6328125" style="6"/>
-    <col min="69" max="69" width="9.6328125" style="9"/>
-    <col min="130" max="130" width="9.6328125" style="11"/>
-    <col min="167" max="167" width="9.6328125" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" style="3"/>
+    <col min="56" max="56" width="9.5703125" style="6"/>
+    <col min="69" max="69" width="9.5703125" style="9"/>
+    <col min="127" max="128" width="12" bestFit="1" customWidth="1"/>
+    <col min="130" max="130" width="9.5703125" style="11"/>
+    <col min="167" max="167" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:181" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:181" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
@@ -1666,7 +1667,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="2" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2175,7 +2176,7 @@
         <v>2.005895263867258</v>
       </c>
     </row>
-    <row r="3" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -2717,7 +2718,7 @@
         <v>1.9457575679140795</v>
       </c>
     </row>
-    <row r="4" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -3244,7 +3245,7 @@
         <v>-1.8523859399617344</v>
       </c>
     </row>
-    <row r="5" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -3777,7 +3778,7 @@
         <v>1.211773157886286</v>
       </c>
     </row>
-    <row r="6" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -4298,7 +4299,7 @@
         <v>0.39906986340708422</v>
       </c>
     </row>
-    <row r="7" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -4834,7 +4835,7 @@
         <v>0.88559368044494735</v>
       </c>
     </row>
-    <row r="8" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -5361,7 +5362,7 @@
         <v>-1.2826825384337934</v>
       </c>
     </row>
-    <row r="9" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -5903,7 +5904,7 @@
         <v>-0.21509390506722759</v>
       </c>
     </row>
-    <row r="10" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -6241,7 +6242,7 @@
         <v>2.6239520958083826</v>
       </c>
       <c r="DW10">
-        <v>1.0958000155267451</v>
+        <v>1.09580001552675</v>
       </c>
       <c r="DX10">
         <v>1.3911963356882229</v>
@@ -6394,7 +6395,7 @@
         <v>1.1314434049639606</v>
       </c>
     </row>
-    <row r="11" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -6880,7 +6881,7 @@
         <v>-0.98115112754233091</v>
       </c>
     </row>
-    <row r="12" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -7255,7 +7256,7 @@
         <v>2.4582718733017623</v>
       </c>
       <c r="DX12">
-        <v>5.5198428290766186</v>
+        <v>5.5198428290766204</v>
       </c>
       <c r="DY12">
         <v>2.7218074656188609</v>
@@ -7417,7 +7418,7 @@
         <v>-0.61773479059422454</v>
       </c>
     </row>
-    <row r="13" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -7923,7 +7924,7 @@
         <v>-1.6774439277104751</v>
       </c>
     </row>
-    <row r="14" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -8468,7 +8469,7 @@
         <v>-0.15173916263016063</v>
       </c>
     </row>
-    <row r="15" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -8995,7 +8996,7 @@
         <v>-1.0468597367484604</v>
       </c>
     </row>
-    <row r="16" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -9522,7 +9523,7 @@
         <v>-1.7529298383114416</v>
       </c>
     </row>
-    <row r="17" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -10058,7 +10059,7 @@
         <v>-1.4472518599047017</v>
       </c>
     </row>
-    <row r="18" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -10588,7 +10589,7 @@
         <v>0.9420078504264402</v>
       </c>
     </row>
-    <row r="19" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -11115,7 +11116,7 @@
         <v>-0.22816029003109295</v>
       </c>
     </row>
-    <row r="20" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -11657,7 +11658,7 @@
         <v>0.57727005508929641</v>
       </c>
     </row>
-    <row r="21" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -12199,7 +12200,7 @@
         <v>-0.515374227778298</v>
       </c>
     </row>
-    <row r="22" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -12744,7 +12745,7 @@
         <v>-1.1825319796615261</v>
       </c>
     </row>
-    <row r="23" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -13268,7 +13269,7 @@
         <v>-1.6211008244408391</v>
       </c>
     </row>
-    <row r="24" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -13810,7 +13811,7 @@
         <v>0.89641490726544015</v>
       </c>
     </row>
-    <row r="25" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -14343,7 +14344,7 @@
         <v>0.97145273795872622</v>
       </c>
     </row>
-    <row r="26" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -14867,7 +14868,7 @@
         <v>0.28102893356779896</v>
       </c>
     </row>
-    <row r="27" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -15409,7 +15410,7 @@
         <v>-1.4351115830189038</v>
       </c>
     </row>
-    <row r="28" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -15951,7 +15952,7 @@
         <v>2.2221157753440104</v>
       </c>
     </row>
-    <row r="29" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -16475,7 +16476,7 @@
         <v>-0.21189241876989418</v>
       </c>
     </row>
-    <row r="30" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -16984,7 +16985,7 @@
         <v>-0.47700819304913333</v>
       </c>
     </row>
-    <row r="31" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -17526,7 +17527,7 @@
         <v>0.41823967432283005</v>
       </c>
     </row>
-    <row r="32" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -18059,7 +18060,7 @@
         <v>1.7015553948875224</v>
       </c>
     </row>
-    <row r="33" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -18583,7 +18584,7 @@
         <v>0.72242101398013647</v>
       </c>
     </row>
-    <row r="34" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -19122,7 +19123,7 @@
         <v>-1.8082968471138963</v>
       </c>
     </row>
-    <row r="35" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -19664,7 +19665,7 @@
         <v>-0.68596517045377992</v>
       </c>
     </row>
-    <row r="36" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -20206,7 +20207,7 @@
         <v>2.712094076416216</v>
       </c>
     </row>
-    <row r="37" spans="1:181" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:181" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -20648,9 +20649,9 @@
       <selection activeCell="A6" sqref="A6:B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -20658,7 +20659,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -20669,7 +20670,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -20680,7 +20681,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>65</v>
       </c>
@@ -20691,7 +20692,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>67</v>
       </c>
@@ -20702,7 +20703,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>69</v>
       </c>
@@ -20713,7 +20714,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>71</v>
       </c>
@@ -20724,7 +20725,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>73</v>
       </c>
@@ -20735,7 +20736,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>75</v>
       </c>
@@ -20746,7 +20747,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>77</v>
       </c>
@@ -20757,7 +20758,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>79</v>
       </c>
@@ -20768,7 +20769,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>80</v>
       </c>
@@ -20779,7 +20780,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>81</v>
       </c>
@@ -20790,7 +20791,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>82</v>
       </c>
@@ -20801,7 +20802,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>84</v>
       </c>

</xml_diff>

<commit_message>
new scripts for true and total triglycerides
</commit_message>
<xml_diff>
--- a/GreenIguanaMasterSpring2021.xlsx
+++ b/GreenIguanaMasterSpring2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usu-my.sharepoint.com/personal/a02308724_aggies_usu_edu/Documents/Desktop/ASU green iguana 2021/greeniguanaAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="329" documentId="8_{D3E1F204-3744-4711-9BBE-5D795E9D066E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B59690EE-2B02-4788-8E1E-52D07A6B640B}"/>
+  <xr:revisionPtr revIDLastSave="332" documentId="8_{D3E1F204-3744-4711-9BBE-5D795E9D066E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4FA4442-8C37-4178-8A06-0CB0DEC4FA79}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-470" windowWidth="19420" windowHeight="10420" xr2:uid="{480D2B5B-0BF7-4EFB-BBDF-5EF1CCA213B8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{480D2B5B-0BF7-4EFB-BBDF-5EF1CCA213B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Assay" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="231">
   <si>
     <t>0324bka</t>
   </si>
@@ -710,6 +710,24 @@
   </si>
   <si>
     <t>l</t>
+  </si>
+  <si>
+    <t>0324cort</t>
+  </si>
+  <si>
+    <t>0423cort</t>
+  </si>
+  <si>
+    <t>0428cort</t>
+  </si>
+  <si>
+    <t>0528cort</t>
+  </si>
+  <si>
+    <t>0624cort</t>
+  </si>
+  <si>
+    <t>0628cort</t>
   </si>
 </sst>
 </file>
@@ -1105,24 +1123,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2963F0F5-C338-45B4-9605-B5DDA288A732}">
-  <dimension ref="A1:FY37"/>
+  <dimension ref="A1:GE37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="CV1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1:E1048576"/>
+      <pane xSplit="1" topLeftCell="FJ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="GD15" sqref="GD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" style="3"/>
-    <col min="56" max="56" width="9.5703125" style="6"/>
-    <col min="69" max="69" width="9.5703125" style="9"/>
+    <col min="1" max="1" width="9.54296875" style="3"/>
+    <col min="56" max="56" width="9.54296875" style="6"/>
+    <col min="69" max="69" width="9.54296875" style="9"/>
     <col min="127" max="128" width="12" bestFit="1" customWidth="1"/>
-    <col min="130" max="130" width="9.5703125" style="11"/>
-    <col min="167" max="167" width="9.5703125" customWidth="1"/>
+    <col min="130" max="130" width="9.54296875" style="11"/>
+    <col min="167" max="167" width="9.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:181" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:187" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
@@ -1666,8 +1684,26 @@
       <c r="FY1" s="3" t="s">
         <v>217</v>
       </c>
+      <c r="FZ1" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="GA1" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="GB1" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="GC1" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="GD1" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="GE1" s="3" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="2" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2175,8 +2211,23 @@
       <c r="FY2">
         <v>2.005895263867258</v>
       </c>
+      <c r="FZ2">
+        <v>44.601999999999997</v>
+      </c>
+      <c r="GA2">
+        <v>22.869</v>
+      </c>
+      <c r="GB2">
+        <v>19.222000000000001</v>
+      </c>
+      <c r="GC2">
+        <v>22.128</v>
+      </c>
+      <c r="GE2">
+        <v>27.312000000000001</v>
+      </c>
     </row>
-    <row r="3" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -2717,8 +2768,23 @@
       <c r="FY3">
         <v>1.9457575679140795</v>
       </c>
+      <c r="FZ3">
+        <v>35.597000000000001</v>
+      </c>
+      <c r="GA3">
+        <v>45.436</v>
+      </c>
+      <c r="GB3">
+        <v>43.259</v>
+      </c>
+      <c r="GC3">
+        <v>40.908999999999999</v>
+      </c>
+      <c r="GD3">
+        <v>30.33</v>
+      </c>
     </row>
-    <row r="4" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -3244,8 +3310,26 @@
       <c r="FY4">
         <v>-1.8523859399617344</v>
       </c>
+      <c r="FZ4">
+        <v>35.825000000000003</v>
+      </c>
+      <c r="GA4">
+        <v>38.889000000000003</v>
+      </c>
+      <c r="GB4">
+        <v>23.172999999999998</v>
+      </c>
+      <c r="GC4">
+        <v>53.816000000000003</v>
+      </c>
+      <c r="GD4">
+        <v>17.481999999999999</v>
+      </c>
+      <c r="GE4">
+        <v>24.004000000000001</v>
+      </c>
     </row>
-    <row r="5" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -3777,8 +3861,26 @@
       <c r="FY5">
         <v>1.211773157886286</v>
       </c>
+      <c r="FZ5">
+        <v>36.130000000000003</v>
+      </c>
+      <c r="GA5">
+        <v>81.99</v>
+      </c>
+      <c r="GB5">
+        <v>55.875999999999998</v>
+      </c>
+      <c r="GC5">
+        <v>38.124000000000002</v>
+      </c>
+      <c r="GD5">
+        <v>23.187000000000001</v>
+      </c>
+      <c r="GE5">
+        <v>27.277000000000001</v>
+      </c>
     </row>
-    <row r="6" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -4298,8 +4400,26 @@
       <c r="FY6">
         <v>0.39906986340708422</v>
       </c>
+      <c r="FZ6">
+        <v>61.947000000000003</v>
+      </c>
+      <c r="GA6">
+        <v>617.96</v>
+      </c>
+      <c r="GB6">
+        <v>190.93700000000001</v>
+      </c>
+      <c r="GC6">
+        <v>56.649000000000001</v>
+      </c>
+      <c r="GD6">
+        <v>96.343999999999994</v>
+      </c>
+      <c r="GE6">
+        <v>71.06</v>
+      </c>
     </row>
-    <row r="7" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -4834,8 +4954,23 @@
       <c r="FY7">
         <v>0.88559368044494735</v>
       </c>
+      <c r="FZ7">
+        <v>61.012999999999998</v>
+      </c>
+      <c r="GA7">
+        <v>73.781999999999996</v>
+      </c>
+      <c r="GC7">
+        <v>44.174999999999997</v>
+      </c>
+      <c r="GD7">
+        <v>31.172999999999998</v>
+      </c>
+      <c r="GE7">
+        <v>25.155999999999999</v>
+      </c>
     </row>
-    <row r="8" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -5361,8 +5496,26 @@
       <c r="FX8">
         <v>-1.2826825384337934</v>
       </c>
+      <c r="FZ8">
+        <v>46.069000000000003</v>
+      </c>
+      <c r="GA8">
+        <v>103.869</v>
+      </c>
+      <c r="GB8">
+        <v>43.094000000000001</v>
+      </c>
+      <c r="GC8">
+        <v>31.172999999999998</v>
+      </c>
+      <c r="GD8">
+        <v>21.966000000000001</v>
+      </c>
+      <c r="GE8">
+        <v>45.673999999999999</v>
+      </c>
     </row>
-    <row r="9" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -5903,8 +6056,26 @@
       <c r="FY9">
         <v>-0.21509390506722759</v>
       </c>
+      <c r="FZ9">
+        <v>8.0239999999999991</v>
+      </c>
+      <c r="GA9">
+        <v>47.831000000000003</v>
+      </c>
+      <c r="GB9">
+        <v>28.376999999999999</v>
+      </c>
+      <c r="GC9">
+        <v>20.76</v>
+      </c>
+      <c r="GD9">
+        <v>24.619</v>
+      </c>
+      <c r="GE9">
+        <v>8.8659999999999997</v>
+      </c>
     </row>
-    <row r="10" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -6394,8 +6565,23 @@
       <c r="FY10">
         <v>1.1314434049639606</v>
       </c>
+      <c r="FZ10">
+        <v>49.122999999999998</v>
+      </c>
+      <c r="GA10">
+        <v>21.63</v>
+      </c>
+      <c r="GB10">
+        <v>20.023</v>
+      </c>
+      <c r="GC10">
+        <v>26.626000000000001</v>
+      </c>
+      <c r="GD10">
+        <v>17.044</v>
+      </c>
     </row>
-    <row r="11" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -6880,8 +7066,23 @@
       <c r="FY11">
         <v>-0.98115112754233091</v>
       </c>
+      <c r="GA11">
+        <v>343.91800000000001</v>
+      </c>
+      <c r="GB11">
+        <v>49.96</v>
+      </c>
+      <c r="GC11">
+        <v>42.136000000000003</v>
+      </c>
+      <c r="GD11">
+        <v>35.890999999999998</v>
+      </c>
+      <c r="GE11">
+        <v>22.978000000000002</v>
+      </c>
     </row>
-    <row r="12" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -7417,8 +7618,26 @@
       <c r="FY12">
         <v>-0.61773479059422454</v>
       </c>
+      <c r="FZ12">
+        <v>92.84</v>
+      </c>
+      <c r="GA12">
+        <v>45.061999999999998</v>
+      </c>
+      <c r="GB12">
+        <v>28.934999999999999</v>
+      </c>
+      <c r="GC12">
+        <v>40.067999999999998</v>
+      </c>
+      <c r="GD12">
+        <v>16.658000000000001</v>
+      </c>
+      <c r="GE12">
+        <v>2.9329999999999998</v>
+      </c>
     </row>
-    <row r="13" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -7923,8 +8142,23 @@
       <c r="FY13">
         <v>-1.6774439277104751</v>
       </c>
+      <c r="FZ13">
+        <v>40.32</v>
+      </c>
+      <c r="GB13">
+        <v>29.384</v>
+      </c>
+      <c r="GC13">
+        <v>39.747999999999998</v>
+      </c>
+      <c r="GD13">
+        <v>25.663</v>
+      </c>
+      <c r="GE13">
+        <v>62.040999999999997</v>
+      </c>
     </row>
-    <row r="14" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -8468,8 +8702,26 @@
       <c r="FY14">
         <v>-0.15173916263016063</v>
       </c>
+      <c r="FZ14">
+        <v>33.835999999999999</v>
+      </c>
+      <c r="GA14">
+        <v>32.911000000000001</v>
+      </c>
+      <c r="GB14">
+        <v>14.132999999999999</v>
+      </c>
+      <c r="GC14">
+        <v>31.966000000000001</v>
+      </c>
+      <c r="GD14">
+        <v>27.614000000000001</v>
+      </c>
+      <c r="GE14">
+        <v>35.308</v>
+      </c>
     </row>
-    <row r="15" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -8995,8 +9247,26 @@
       <c r="FY15">
         <v>-1.0468597367484604</v>
       </c>
+      <c r="FZ15">
+        <v>31.407</v>
+      </c>
+      <c r="GA15">
+        <v>27.88</v>
+      </c>
+      <c r="GB15">
+        <v>18.093</v>
+      </c>
+      <c r="GC15">
+        <v>31.51</v>
+      </c>
+      <c r="GD15">
+        <v>31.611999999999998</v>
+      </c>
+      <c r="GE15">
+        <v>26.593</v>
+      </c>
     </row>
-    <row r="16" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -9522,8 +9792,26 @@
       <c r="FY16">
         <v>-1.7529298383114416</v>
       </c>
+      <c r="FZ16">
+        <v>32.581000000000003</v>
+      </c>
+      <c r="GA16">
+        <v>18.34</v>
+      </c>
+      <c r="GB16">
+        <v>28.518999999999998</v>
+      </c>
+      <c r="GC16">
+        <v>33.421999999999997</v>
+      </c>
+      <c r="GD16">
+        <v>16.943999999999999</v>
+      </c>
+      <c r="GE16">
+        <v>27.484000000000002</v>
+      </c>
     </row>
-    <row r="17" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -10058,8 +10346,26 @@
       <c r="FY17">
         <v>-1.4472518599047017</v>
       </c>
+      <c r="FZ17">
+        <v>58.75</v>
+      </c>
+      <c r="GA17">
+        <v>53.81</v>
+      </c>
+      <c r="GB17">
+        <v>48.872</v>
+      </c>
+      <c r="GC17">
+        <v>31.567</v>
+      </c>
+      <c r="GD17">
+        <v>37.987000000000002</v>
+      </c>
+      <c r="GE17">
+        <v>40.064</v>
+      </c>
     </row>
-    <row r="18" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -10588,8 +10894,26 @@
       <c r="FY18">
         <v>0.9420078504264402</v>
       </c>
+      <c r="FZ18">
+        <v>35.308</v>
+      </c>
+      <c r="GA18">
+        <v>12.595000000000001</v>
+      </c>
+      <c r="GB18">
+        <v>11.52</v>
+      </c>
+      <c r="GC18">
+        <v>20.492999999999999</v>
+      </c>
+      <c r="GD18">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="GE18">
+        <v>24.794</v>
+      </c>
     </row>
-    <row r="19" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -11115,8 +11439,23 @@
       <c r="FY19">
         <v>-0.22816029003109295</v>
       </c>
+      <c r="FZ19">
+        <v>45.41</v>
+      </c>
+      <c r="GB19">
+        <v>114.414</v>
+      </c>
+      <c r="GC19">
+        <v>57.173000000000002</v>
+      </c>
+      <c r="GD19">
+        <v>39.747999999999998</v>
+      </c>
+      <c r="GE19">
+        <v>48.494999999999997</v>
+      </c>
     </row>
-    <row r="20" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -11657,8 +11996,26 @@
       <c r="FY20">
         <v>0.57727005508929641</v>
       </c>
+      <c r="FZ20">
+        <v>31.34</v>
+      </c>
+      <c r="GA20">
+        <v>19.562000000000001</v>
+      </c>
+      <c r="GB20">
+        <v>30.437999999999999</v>
+      </c>
+      <c r="GC20">
+        <v>22.56</v>
+      </c>
+      <c r="GD20">
+        <v>24.141999999999999</v>
+      </c>
+      <c r="GE20">
+        <v>40.728000000000002</v>
+      </c>
     </row>
-    <row r="21" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -12199,8 +12556,26 @@
       <c r="FY21">
         <v>-0.515374227778298</v>
       </c>
+      <c r="FZ21">
+        <v>35.134999999999998</v>
+      </c>
+      <c r="GA21">
+        <v>61.424999999999997</v>
+      </c>
+      <c r="GB21">
+        <v>30.992999999999999</v>
+      </c>
+      <c r="GC21">
+        <v>35.89</v>
+      </c>
+      <c r="GD21">
+        <v>23.963000000000001</v>
+      </c>
+      <c r="GE21">
+        <v>43.4</v>
+      </c>
     </row>
-    <row r="22" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -12744,8 +13119,26 @@
       <c r="FY22">
         <v>-1.1825319796615261</v>
       </c>
+      <c r="FZ22">
+        <v>72.257999999999996</v>
+      </c>
+      <c r="GA22">
+        <v>31.57</v>
+      </c>
+      <c r="GB22">
+        <v>40.695999999999998</v>
+      </c>
+      <c r="GC22">
+        <v>49.96</v>
+      </c>
+      <c r="GD22">
+        <v>1.92</v>
+      </c>
+      <c r="GE22">
+        <v>38.869999999999997</v>
+      </c>
     </row>
-    <row r="23" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -13268,8 +13661,26 @@
       <c r="FY23">
         <v>-1.6211008244408391</v>
       </c>
+      <c r="FZ23">
+        <v>48.185000000000002</v>
+      </c>
+      <c r="GA23">
+        <v>26.361999999999998</v>
+      </c>
+      <c r="GB23">
+        <v>38.65</v>
+      </c>
+      <c r="GC23">
+        <v>35.616</v>
+      </c>
+      <c r="GD23">
+        <v>29.847000000000001</v>
+      </c>
+      <c r="GE23">
+        <v>26.725000000000001</v>
+      </c>
     </row>
-    <row r="24" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -13810,8 +14221,26 @@
       <c r="FY24">
         <v>0.89641490726544015</v>
       </c>
+      <c r="FZ24">
+        <v>75</v>
+      </c>
+      <c r="GA24">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="GB24">
+        <v>36.363999999999997</v>
+      </c>
+      <c r="GC24">
+        <v>34.667000000000002</v>
+      </c>
+      <c r="GD24">
+        <v>23.821999999999999</v>
+      </c>
+      <c r="GE24">
+        <v>42.515999999999998</v>
+      </c>
     </row>
-    <row r="25" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -14343,8 +14772,23 @@
       <c r="FY25">
         <v>0.97145273795872622</v>
       </c>
+      <c r="FZ25">
+        <v>37.741999999999997</v>
+      </c>
+      <c r="GA25">
+        <v>29.16</v>
+      </c>
+      <c r="GB25">
+        <v>65.162000000000006</v>
+      </c>
+      <c r="GD25">
+        <v>13.396000000000001</v>
+      </c>
+      <c r="GE25">
+        <v>21.434000000000001</v>
+      </c>
     </row>
-    <row r="26" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -14867,8 +15311,26 @@
       <c r="FY26">
         <v>0.28102893356779896</v>
       </c>
+      <c r="FZ26">
+        <v>36.908999999999999</v>
+      </c>
+      <c r="GA26">
+        <v>45.768000000000001</v>
+      </c>
+      <c r="GB26">
+        <v>50.783000000000001</v>
+      </c>
+      <c r="GC26">
+        <v>29.925999999999998</v>
+      </c>
+      <c r="GD26">
+        <v>24.808</v>
+      </c>
+      <c r="GE26">
+        <v>49.96</v>
+      </c>
     </row>
-    <row r="27" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -15409,8 +15871,26 @@
       <c r="FY27">
         <v>-1.4351115830189038</v>
       </c>
+      <c r="FZ27">
+        <v>160.32900000000001</v>
+      </c>
+      <c r="GA27">
+        <v>6.798</v>
+      </c>
+      <c r="GB27">
+        <v>60.106999999999999</v>
+      </c>
+      <c r="GC27">
+        <v>48.185000000000002</v>
+      </c>
+      <c r="GD27">
+        <v>25.29</v>
+      </c>
+      <c r="GE27">
+        <v>27.984999999999999</v>
+      </c>
     </row>
-    <row r="28" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -15951,8 +16431,26 @@
       <c r="FY28">
         <v>2.2221157753440104</v>
       </c>
+      <c r="FZ28">
+        <v>57.082999999999998</v>
+      </c>
+      <c r="GA28">
+        <v>30.56</v>
+      </c>
+      <c r="GB28">
+        <v>28.411000000000001</v>
+      </c>
+      <c r="GC28">
+        <v>43.523000000000003</v>
+      </c>
+      <c r="GD28">
+        <v>35.89</v>
+      </c>
+      <c r="GE28">
+        <v>50.685000000000002</v>
+      </c>
     </row>
-    <row r="29" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -16475,8 +16973,26 @@
       <c r="FY29">
         <v>-0.21189241876989418</v>
       </c>
+      <c r="FZ29">
+        <v>46.423000000000002</v>
+      </c>
+      <c r="GA29">
+        <v>28.571000000000002</v>
+      </c>
+      <c r="GB29">
+        <v>56.228999999999999</v>
+      </c>
+      <c r="GC29">
+        <v>37.987000000000002</v>
+      </c>
+      <c r="GD29">
+        <v>21.553000000000001</v>
+      </c>
+      <c r="GE29">
+        <v>25.353000000000002</v>
+      </c>
     </row>
-    <row r="30" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -16984,8 +17500,26 @@
       <c r="FX30">
         <v>-0.47700819304913333</v>
       </c>
+      <c r="FZ30">
+        <v>35.081000000000003</v>
+      </c>
+      <c r="GA30">
+        <v>22.036999999999999</v>
+      </c>
+      <c r="GB30">
+        <v>30.547999999999998</v>
+      </c>
+      <c r="GC30">
+        <v>32.276000000000003</v>
+      </c>
+      <c r="GD30">
+        <v>12.224</v>
+      </c>
+      <c r="GE30">
+        <v>19.452999999999999</v>
+      </c>
     </row>
-    <row r="31" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -17526,8 +18060,26 @@
       <c r="FY31">
         <v>0.41823967432283005</v>
       </c>
+      <c r="FZ31">
+        <v>55.131999999999998</v>
+      </c>
+      <c r="GA31">
+        <v>0.73799999999999999</v>
+      </c>
+      <c r="GB31">
+        <v>37.838000000000001</v>
+      </c>
+      <c r="GC31">
+        <v>1.484</v>
+      </c>
+      <c r="GD31">
+        <v>37.44</v>
+      </c>
+      <c r="GE31">
+        <v>47.402999999999999</v>
+      </c>
     </row>
-    <row r="32" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -18059,8 +18611,26 @@
       <c r="FY32">
         <v>1.7015553948875224</v>
       </c>
+      <c r="FZ32">
+        <v>31.661000000000001</v>
+      </c>
+      <c r="GA32">
+        <v>7.665</v>
+      </c>
+      <c r="GB32">
+        <v>23.55</v>
+      </c>
+      <c r="GC32">
+        <v>30.56</v>
+      </c>
+      <c r="GD32">
+        <v>31.414999999999999</v>
+      </c>
+      <c r="GE32">
+        <v>23.55</v>
+      </c>
     </row>
-    <row r="33" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -18583,8 +19153,26 @@
       <c r="FY33">
         <v>0.72242101398013647</v>
       </c>
+      <c r="FZ33">
+        <v>46.423000000000002</v>
+      </c>
+      <c r="GA33">
+        <v>39.762</v>
+      </c>
+      <c r="GB33">
+        <v>174.70500000000001</v>
+      </c>
+      <c r="GC33">
+        <v>44.761000000000003</v>
+      </c>
+      <c r="GD33">
+        <v>43.003999999999998</v>
+      </c>
+      <c r="GE33">
+        <v>36.99</v>
+      </c>
     </row>
-    <row r="34" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -19122,8 +19710,26 @@
       <c r="FY34">
         <v>-1.8082968471138963</v>
       </c>
+      <c r="FZ34">
+        <v>35.439</v>
+      </c>
+      <c r="GA34">
+        <v>62.76</v>
+      </c>
+      <c r="GB34">
+        <v>49.96</v>
+      </c>
+      <c r="GC34">
+        <v>147.86199999999999</v>
+      </c>
+      <c r="GD34">
+        <v>51.015000000000001</v>
+      </c>
+      <c r="GE34">
+        <v>49.241</v>
+      </c>
     </row>
-    <row r="35" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -19664,8 +20270,26 @@
       <c r="FY35">
         <v>-0.68596517045377992</v>
       </c>
+      <c r="FZ35">
+        <v>60.106999999999999</v>
+      </c>
+      <c r="GA35">
+        <v>818.33100000000002</v>
+      </c>
+      <c r="GB35">
+        <v>56.649000000000001</v>
+      </c>
+      <c r="GC35">
+        <v>35.134999999999998</v>
+      </c>
+      <c r="GD35">
+        <v>42.085999999999999</v>
+      </c>
+      <c r="GE35">
+        <v>30.745999999999999</v>
+      </c>
     </row>
-    <row r="36" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -20206,8 +20830,26 @@
       <c r="FY36">
         <v>2.712094076416216</v>
       </c>
+      <c r="FZ36">
+        <v>21.904</v>
+      </c>
+      <c r="GA36">
+        <v>26.521000000000001</v>
+      </c>
+      <c r="GB36">
+        <v>70.635000000000005</v>
+      </c>
+      <c r="GC36">
+        <v>30</v>
+      </c>
+      <c r="GD36">
+        <v>40.484999999999999</v>
+      </c>
+      <c r="GE36">
+        <v>48.911000000000001</v>
+      </c>
     </row>
-    <row r="37" spans="1:181" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:187" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -20633,6 +21275,18 @@
       </c>
       <c r="FX37">
         <v>-1.1350963485906889</v>
+      </c>
+      <c r="FZ37">
+        <v>40.645000000000003</v>
+      </c>
+      <c r="GA37">
+        <v>18.138999999999999</v>
+      </c>
+      <c r="GC37">
+        <v>71.921000000000006</v>
+      </c>
+      <c r="GD37">
+        <v>25.29</v>
       </c>
     </row>
   </sheetData>
@@ -20649,9 +21303,9 @@
       <selection activeCell="A6" sqref="A6:B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -20659,7 +21313,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -20670,7 +21324,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -20681,7 +21335,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>65</v>
       </c>
@@ -20692,7 +21346,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>67</v>
       </c>
@@ -20703,7 +21357,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>69</v>
       </c>
@@ -20714,7 +21368,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>71</v>
       </c>
@@ -20725,7 +21379,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>73</v>
       </c>
@@ -20736,7 +21390,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>75</v>
       </c>
@@ -20747,7 +21401,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>77</v>
       </c>
@@ -20758,7 +21412,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>79</v>
       </c>
@@ -20769,7 +21423,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>80</v>
       </c>
@@ -20780,7 +21434,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>81</v>
       </c>
@@ -20791,7 +21445,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>82</v>
       </c>
@@ -20802,7 +21456,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>84</v>
       </c>

</xml_diff>

<commit_message>
start glucose 3 month effect analysis
</commit_message>
<xml_diff>
--- a/GreenIguanaMasterSpring2021.xlsx
+++ b/GreenIguanaMasterSpring2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usu-my.sharepoint.com/personal/a02308724_aggies_usu_edu/Documents/Desktop/ASU green iguana 2021/greeniguanaAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="332" documentId="8_{D3E1F204-3744-4711-9BBE-5D795E9D066E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4FA4442-8C37-4178-8A06-0CB0DEC4FA79}"/>
+  <xr:revisionPtr revIDLastSave="334" documentId="8_{D3E1F204-3744-4711-9BBE-5D795E9D066E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FD3F749-5F7B-4E6D-9746-8E0148573FA6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{480D2B5B-0BF7-4EFB-BBDF-5EF1CCA213B8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{480D2B5B-0BF7-4EFB-BBDF-5EF1CCA213B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Assay" sheetId="2" r:id="rId1"/>
@@ -1127,20 +1127,20 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="FJ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="GD15" sqref="GD15"/>
+      <selection pane="topRight" activeCell="FP14" sqref="A1:GE37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.54296875" style="3"/>
-    <col min="56" max="56" width="9.54296875" style="6"/>
-    <col min="69" max="69" width="9.54296875" style="9"/>
+    <col min="1" max="1" width="9.5703125" style="3"/>
+    <col min="56" max="56" width="9.5703125" style="6"/>
+    <col min="69" max="69" width="9.5703125" style="9"/>
     <col min="127" max="128" width="12" bestFit="1" customWidth="1"/>
-    <col min="130" max="130" width="9.54296875" style="11"/>
-    <col min="167" max="167" width="9.54296875" customWidth="1"/>
+    <col min="130" max="130" width="9.5703125" style="11"/>
+    <col min="167" max="167" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:187" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:187" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="2" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>27.312000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -2784,7 +2784,7 @@
         <v>30.33</v>
       </c>
     </row>
-    <row r="4" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -3329,7 +3329,7 @@
         <v>24.004000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -3880,7 +3880,7 @@
         <v>27.277000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -4419,7 +4419,7 @@
         <v>71.06</v>
       </c>
     </row>
-    <row r="7" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -4970,7 +4970,7 @@
         <v>25.155999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -5515,7 +5515,7 @@
         <v>45.673999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -6075,7 +6075,7 @@
         <v>8.8659999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -6581,7 +6581,7 @@
         <v>17.044</v>
       </c>
     </row>
-    <row r="11" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -7082,7 +7082,7 @@
         <v>22.978000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -7637,7 +7637,7 @@
         <v>2.9329999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -8158,7 +8158,7 @@
         <v>62.040999999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -8721,7 +8721,7 @@
         <v>35.308</v>
       </c>
     </row>
-    <row r="15" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -9266,7 +9266,7 @@
         <v>26.593</v>
       </c>
     </row>
-    <row r="16" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -9811,7 +9811,7 @@
         <v>27.484000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -10365,7 +10365,7 @@
         <v>40.064</v>
       </c>
     </row>
-    <row r="18" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -10913,7 +10913,7 @@
         <v>24.794</v>
       </c>
     </row>
-    <row r="19" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -11455,7 +11455,7 @@
         <v>48.494999999999997</v>
       </c>
     </row>
-    <row r="20" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -12015,7 +12015,7 @@
         <v>40.728000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -12575,7 +12575,7 @@
         <v>43.4</v>
       </c>
     </row>
-    <row r="22" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -13138,7 +13138,7 @@
         <v>38.869999999999997</v>
       </c>
     </row>
-    <row r="23" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -13680,7 +13680,7 @@
         <v>26.725000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -14240,7 +14240,7 @@
         <v>42.515999999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -14788,7 +14788,7 @@
         <v>21.434000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -15330,7 +15330,7 @@
         <v>49.96</v>
       </c>
     </row>
-    <row r="27" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -15890,7 +15890,7 @@
         <v>27.984999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -16450,7 +16450,7 @@
         <v>50.685000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -16992,7 +16992,7 @@
         <v>25.353000000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -17519,7 +17519,7 @@
         <v>19.452999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -18079,7 +18079,7 @@
         <v>47.402999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -18630,7 +18630,7 @@
         <v>23.55</v>
       </c>
     </row>
-    <row r="33" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -19172,7 +19172,7 @@
         <v>36.99</v>
       </c>
     </row>
-    <row r="34" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -19729,7 +19729,7 @@
         <v>49.241</v>
       </c>
     </row>
-    <row r="35" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -20289,7 +20289,7 @@
         <v>30.745999999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -20849,7 +20849,7 @@
         <v>48.911000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:187" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:187" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -21303,9 +21303,9 @@
       <selection activeCell="A6" sqref="A6:B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -21313,7 +21313,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -21324,7 +21324,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -21335,7 +21335,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>65</v>
       </c>
@@ -21346,7 +21346,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>67</v>
       </c>
@@ -21357,7 +21357,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>69</v>
       </c>
@@ -21368,7 +21368,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>71</v>
       </c>
@@ -21379,7 +21379,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>73</v>
       </c>
@@ -21390,7 +21390,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>75</v>
       </c>
@@ -21401,7 +21401,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>77</v>
       </c>
@@ -21412,7 +21412,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>79</v>
       </c>
@@ -21423,7 +21423,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>80</v>
       </c>
@@ -21434,7 +21434,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>81</v>
       </c>
@@ -21445,7 +21445,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>82</v>
       </c>
@@ -21456,7 +21456,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>84</v>
       </c>

</xml_diff>